<commit_message>
finalised pokemon data for now
</commit_message>
<xml_diff>
--- a/Content/_Data/Pokemon/pokemon-data.xlsx
+++ b/Content/_Data/Pokemon/pokemon-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Unreal\PokemonRemake\Content\_Data\Pokemon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{522E2C78-4990-4FA5-9954-F73B3561901B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCD65155-4AC2-4BE3-99D8-8FC1CB489060}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="259">
   <si>
     <t>Alien</t>
   </si>
@@ -501,9 +501,6 @@
     <t>Stomach Pokemon</t>
   </si>
   <si>
-    <t xml:space="preserve"> 	It has a small heart and brain. Its stomach comprises most of its body, with enzymes to dissolve anything.</t>
-  </si>
-  <si>
     <t>It swallows anything whole. It sweats toxic fluids from its follicles to douse foes.</t>
   </si>
   <si>
@@ -588,33 +585,18 @@
     <t>Prankster</t>
   </si>
   <si>
-    <t>Each Ungaring paints its own individual pattern, and it will paint that same pattern over and over again throughout its life.</t>
-  </si>
-  <si>
     <t>Magic Bounce</t>
   </si>
   <si>
     <t>Dimensional Breach</t>
   </si>
   <si>
-    <t>Legends say their touch can bridge the gap between realities,</t>
-  </si>
-  <si>
-    <t>While some believe Graplinth can freely navigate between dimensions,</t>
-  </si>
-  <si>
-    <t>They're known for their constant chirping,</t>
-  </si>
-  <si>
     <t>Their chirping evolves into a more complex song, some believe it contains hidden messages or carries good luck.</t>
   </si>
   <si>
     <t>Early Bird</t>
   </si>
   <si>
-    <t>Cactoro are surprisingly social creatures,</t>
-  </si>
-  <si>
     <t>Drought</t>
   </si>
   <si>
@@ -624,27 +606,15 @@
     <t>Torrent</t>
   </si>
   <si>
-    <t>Despite their unassuming appearance,</t>
-  </si>
-  <si>
     <t>Blobstrike are agile predators, using their strong arms to propel themselves through the water at surprising speeds and their tails to deliver powerful blows.</t>
   </si>
   <si>
-    <t>Snowti are playful creatures,</t>
-  </si>
-  <si>
-    <t>They are incredibly strong and resilient,</t>
-  </si>
-  <si>
     <t>Snow Cloak</t>
   </si>
   <si>
     <t>Slush Rush</t>
   </si>
   <si>
-    <t>Ninjub are masters of stealth,</t>
-  </si>
-  <si>
     <t>Their loyalty to their trainers deepens with evolution, and they are willing to take any blow meant for their companions.</t>
   </si>
   <si>
@@ -660,51 +630,30 @@
     <t>They are surprisingly fast for their size and fiercely defend their territory from any perceived threats.</t>
   </si>
   <si>
-    <t>Grorc are the soldiers of orc communities,</t>
-  </si>
-  <si>
     <t>Their swings carry the force of a battering ram, and their battle cry can strike fear into the hearts of even the most courageous opponents.</t>
   </si>
   <si>
-    <t>Despite their perpetually tearful appearance,</t>
-  </si>
-  <si>
     <t>Friend Guard</t>
   </si>
   <si>
-    <t>Whistleweep are playful creatures,</t>
-  </si>
-  <si>
     <t>Tailwind</t>
   </si>
   <si>
     <t>Cloud Rider</t>
   </si>
   <si>
-    <t>Combalpa are the undisputed rulers of the skies,</t>
-  </si>
-  <si>
     <t>Sky Majesty</t>
   </si>
   <si>
     <t>Honey Gather</t>
   </si>
   <si>
-    <t>Been are incredibly social creatures,</t>
-  </si>
-  <si>
     <t>They work alongside Been in their hives, collecting pollen and defending their home from predators.</t>
   </si>
   <si>
     <t>Swarm</t>
   </si>
   <si>
-    <t>Dimp are drawn to negative emotions,</t>
-  </si>
-  <si>
-    <t>Dreamon are masters of illusion,</t>
-  </si>
-  <si>
     <t>Frighten</t>
   </si>
   <si>
@@ -720,21 +669,12 @@
     <t>Blaze</t>
   </si>
   <si>
-    <t>Chragon are powerful and majestic creatures,</t>
-  </si>
-  <si>
     <t>Levitate</t>
   </si>
   <si>
-    <t>Gosty are known for their love of pranks,</t>
-  </si>
-  <si>
     <t>While not inherently malicious, Gostaunt can be mischievous and may drain a bit more energy than intended, leaving their victims feeling weak and disoriented.</t>
   </si>
   <si>
-    <t>lub attach themselves to unsuspecting creatures using their powerful suckers,</t>
-  </si>
-  <si>
     <t>Plonster are not only parasitic but also feed on the negative emotions of others, growing stronger with despair and misery.</t>
   </si>
   <si>
@@ -750,36 +690,9 @@
     <t>Sand Veil</t>
   </si>
   <si>
-    <t>Kingapark are the undisputed rulers of the caves they inhabit,</t>
-  </si>
-  <si>
     <t>Sand Rush</t>
   </si>
   <si>
-    <t>Their purrs emit psychic waves that can calm emotions or even induce headaches in those they dislike.</t>
-  </si>
-  <si>
-    <t>Their barks sound like thunderclaps.</t>
-  </si>
-  <si>
-    <t>They love hiding decorated eggs (real or energy-based) for others to find.</t>
-  </si>
-  <si>
-    <t>Bonkster are powerful fighters with ice-covered fur and horns. They fiercely defend their territory.</t>
-  </si>
-  <si>
-    <t>They breathe fire hotter than molten lava.</t>
-  </si>
-  <si>
-    <t>They can generate powerful electric shocks while swimming.</t>
-  </si>
-  <si>
-    <t>They throw toxic berries at their opponents and hide amongst boulders.</t>
-  </si>
-  <si>
-    <t>They inhabit abandoned buildings and feed off negative emotions.</t>
-  </si>
-  <si>
     <t>Cursed Body</t>
   </si>
   <si>
@@ -808,6 +721,99 @@
   </si>
   <si>
     <t>If this Pokemon senses a strong emotion, it will run away as fast as it can. It prefers areas without people.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> It has a small heart and brain. Its stomach comprises most of its body, with enzymes to dissolve anything.</t>
+  </si>
+  <si>
+    <t>Legends say their touch can bridge the gap between realities, though some unfortunate souls claim it merely steals their memories.</t>
+  </si>
+  <si>
+    <t>While some believe Graplinth can freely navigate between dimensions,  others fear it heralds the collapse of the veil separating realities.</t>
+  </si>
+  <si>
+    <t>They're known for their constant chirping, which some find melodic while others find it incessant.</t>
+  </si>
+  <si>
+    <t>Cactoro are surprisingly social creatures, often gathering in groups to conserve moisture and share nutrients.</t>
+  </si>
+  <si>
+    <t>Despite their unassuming appearance, Blobbin are surprisingly resilient and can withstand changes in water pressure with ease.</t>
+  </si>
+  <si>
+    <t>Snowti are playful creatures, often rolling down snowy hills and leaving trails of laughter in their wake.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> They are incredibly strong and resilient, able to withstand harsh blizzards and frigid temperatures. </t>
+  </si>
+  <si>
+    <t>Ninjub are masters of stealth, able to blend into shadows and disappear in an instant.</t>
+  </si>
+  <si>
+    <t>Grorc are the soldiers of orc communities, fiercely loyal and rigorously trained in combat.</t>
+  </si>
+  <si>
+    <t>Despite their perpetually tearful appearance, Weepin are not sad Pokémon.  In fact, their tears are believed to possess healing properties, and Weepin will readily cry on a trainer's wounds to help them mend.</t>
+  </si>
+  <si>
+    <t>Whistleweep are playful creatures, often soaring through the air and leaving trails of shimmering pearls in their wake.</t>
+  </si>
+  <si>
+    <t>Combalpa are the undisputed rulers of the skies, their presence commanding respect from even the most territorial of flying Pokémon.</t>
+  </si>
+  <si>
+    <t>Been are incredibly social creatures, living in large hives and working together to gather pollen and care for their young.</t>
+  </si>
+  <si>
+    <t>Dimp are drawn to negative emotions, feeding off them to grow stronger. They often play cruel pranks, manipulating people's fears and insecurities for their own amusement.</t>
+  </si>
+  <si>
+    <t>Dreamon are masters of illusion, capable of manipulating dreams and creating powerful nightmares. They feed on the terror they inflict, growing stronger with each terrified scream.</t>
+  </si>
+  <si>
+    <t>Chragon are powerful and majestic creatures, capable of unleashing devastating blasts of fire. While still playful at heart, Chragon commands respect with its newfound power.</t>
+  </si>
+  <si>
+    <t>Gosty are known for their love of pranks, often flickering lights, rearranging objects, and giggling as they vanish into thin air. Despite their playful demeanor, Gosty can be accidentally disruptive, and some people find their presence unsettling.</t>
+  </si>
+  <si>
+    <t>Plub attach themselves to unsuspecting creatures using their powerful suckers, draining them of nutrients and leaving them feeling sluggish.</t>
+  </si>
+  <si>
+    <t>Kingapark are the undisputed rulers of the caves they inhabit, fiercely protecting their territory from intruders.</t>
+  </si>
+  <si>
+    <t>A rhythmic purr is their constant companion, and some believe these purrs emit psychic waves that can calm emotions or even induce headaches in those Meow dislikes.</t>
+  </si>
+  <si>
+    <t>Yapper come in a variety of breeds, but all share the same boundless energy and electrifying presence.  They love to chase after rolling objects, and their playful nips can deliver a surprising jolt.</t>
+  </si>
+  <si>
+    <t>Easter have a natural talent for finding hidden objects, and they love hiding decorated eggs (sometimes filled with delicious treats, sometimes filled with energy blasts!) for others to find.</t>
+  </si>
+  <si>
+    <t>Bonkster are fiercely territorial and will defend their homes with brutal efficiency. Despite their intimidating appearance, Bonkster retain a playful streak, often challenging worthy opponents to sparring matches in the snow.</t>
+  </si>
+  <si>
+    <t>A fiery furnace burns within Tyranno's chest, and they can unleash jets of molten lava from their mouths.  The ground trembles with each of their earth-shattering steps, and their mighty roar can send shivers down the spine of even the bravest trainer.</t>
+  </si>
+  <si>
+    <t>Gribspark can leap great distances from the water, leaving a trail of crackling electricity in their wake.</t>
+  </si>
+  <si>
+    <t>Monkroose are surprisingly strong for their size and can hurl rocks with surprising accuracy. They also possess toxic glands that can coat their claws with a potent venom.</t>
+  </si>
+  <si>
+    <t>While rarely seen by human eyes, Ungaring leave behind strange symbols carved into rocks or trees, messages only those attuned to the spirits can understand.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hywirl are drawn to places filled with negative emotions, feeding off despair, anger, and sorrow.  They can manipulate these emotions, amplifying them and driving those around them to madness. </t>
+  </si>
+  <si>
+    <t>Mold Breaker</t>
+  </si>
+  <si>
+    <t>Rock Head</t>
   </si>
 </sst>
 </file>
@@ -1255,8 +1261,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55723188-F4D3-4EF4-AEA8-7A04D3578F8F}">
   <dimension ref="A1:V50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q2" sqref="Q2"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1264,7 +1270,7 @@
     <col min="2" max="2" width="20.28515625" customWidth="1"/>
     <col min="3" max="4" width="22.28515625" customWidth="1"/>
     <col min="7" max="7" width="21.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.85546875" customWidth="1"/>
+    <col min="8" max="8" width="199.85546875" customWidth="1"/>
     <col min="9" max="9" width="14" customWidth="1"/>
     <col min="11" max="11" width="27.42578125" customWidth="1"/>
     <col min="12" max="12" width="22" bestFit="1" customWidth="1"/>
@@ -1303,7 +1309,7 @@
         <v>56</v>
       </c>
       <c r="J1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="K1" t="s">
         <v>102</v>
@@ -1362,21 +1368,21 @@
         <v>79</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H2" t="s">
-        <v>186</v>
+        <v>229</v>
       </c>
       <c r="I2" s="9">
         <f ca="1">ROUND(RAND()*(0.6-0.3)+0.3, 2)</f>
-        <v>0.53</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="J2" s="9">
         <f ca="1">ROUND(RAND()*(10 -1)+1,2)</f>
-        <v>7.84</v>
+        <v>6.93</v>
       </c>
       <c r="K2" s="9" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="L2" s="9" t="s">
         <v>17</v>
@@ -1420,21 +1426,21 @@
         <v>79</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H3" t="s">
-        <v>187</v>
+        <v>230</v>
       </c>
       <c r="I3" s="10">
         <f ca="1">ROUND(RAND()*(2-VALUE(I2))+VALUE(I2),2)</f>
-        <v>1.35</v>
+        <v>0.75</v>
       </c>
       <c r="J3" s="10">
         <f ca="1">ROUND(RAND()*(100-VALUE(J2))+VALUE(J2),2)</f>
-        <v>94.96</v>
+        <v>52.04</v>
       </c>
       <c r="K3" s="9" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="L3" s="10" t="s">
         <v>68</v>
@@ -1478,21 +1484,21 @@
         <v>72</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H4" t="s">
-        <v>188</v>
+        <v>231</v>
       </c>
       <c r="I4" s="9">
         <f ca="1">ROUND(RAND()*(0.6-0.3)+0.3, 2)</f>
-        <v>0.52</v>
+        <v>0.49</v>
       </c>
       <c r="J4" s="9">
         <f ca="1">ROUND(RAND()*(10 -1)+1,2)</f>
-        <v>9.56</v>
+        <v>1.94</v>
       </c>
       <c r="K4" s="9" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="L4" s="9" t="s">
         <v>18</v>
@@ -1536,21 +1542,21 @@
         <v>72</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H5" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="I5" s="10">
         <f ca="1">ROUND(RAND()*(2-VALUE(I4))+VALUE(I4),2)</f>
-        <v>1.34</v>
+        <v>1.37</v>
       </c>
       <c r="J5" s="10">
         <f ca="1">ROUND(RAND()*(100-VALUE(J4))+VALUE(J4),2)</f>
-        <v>95.41</v>
+        <v>87.34</v>
       </c>
       <c r="K5" s="9" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="L5" s="10" t="s">
         <v>68</v>
@@ -1594,21 +1600,21 @@
         <v>68</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="H6" t="s">
-        <v>191</v>
+        <v>232</v>
       </c>
       <c r="I6" s="9">
         <f ca="1">ROUND(RAND()*(0.8-0.3)+0.3, 2)</f>
-        <v>0.65</v>
+        <v>0.66</v>
       </c>
       <c r="J6" s="9">
         <f ca="1">ROUND(RAND()*(10 -1)+1,2)</f>
-        <v>8.49</v>
+        <v>4.18</v>
       </c>
       <c r="K6" s="9" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="L6" s="9" t="s">
         <v>21</v>
@@ -1652,21 +1658,21 @@
         <v>74</v>
       </c>
       <c r="G7" s="10" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="H7" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="I7" s="10">
         <f ca="1">ROUND(RAND()*(2-VALUE(I6))+VALUE(I6),2)</f>
-        <v>1.81</v>
+        <v>1.85</v>
       </c>
       <c r="J7" s="10">
         <f ca="1">ROUND(RAND()*(100-VALUE(J6))+VALUE(J6),2)</f>
-        <v>72.569999999999993</v>
+        <v>67.400000000000006</v>
       </c>
       <c r="K7" s="9" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="L7" s="10" t="s">
         <v>68</v>
@@ -1710,21 +1716,21 @@
         <v>68</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="H8" t="s">
-        <v>195</v>
+        <v>233</v>
       </c>
       <c r="I8" s="9">
         <f ca="1">ROUND(RAND()*(0.5-0.3)+0.3, 2)</f>
-        <v>0.38</v>
+        <v>0.4</v>
       </c>
       <c r="J8" s="9">
         <f ca="1">ROUND(RAND()*(10 -1)+1,2)</f>
-        <v>8.2799999999999994</v>
+        <v>8.6</v>
       </c>
       <c r="K8" s="9" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="L8" s="9" t="s">
         <v>24</v>
@@ -1768,21 +1774,21 @@
         <v>68</v>
       </c>
       <c r="G9" s="10" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H9" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="I9" s="10">
         <f ca="1">ROUND(RAND()*(2-VALUE(I8))+VALUE(I8),2)</f>
-        <v>0.9</v>
+        <v>0.7</v>
       </c>
       <c r="J9" s="10">
         <f ca="1">ROUND(RAND()*(100-VALUE(J8))+VALUE(J8),2)</f>
-        <v>42.04</v>
+        <v>17.36</v>
       </c>
       <c r="K9" s="9" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="L9" s="10" t="s">
         <v>68</v>
@@ -1829,17 +1835,17 @@
         <v>153</v>
       </c>
       <c r="H10" s="9" t="s">
-        <v>154</v>
+        <v>228</v>
       </c>
       <c r="I10" s="9">
         <f ca="1">ROUND(RAND()*(0.5-0.3)+0.3, 2)</f>
-        <v>0.42</v>
+        <v>0.43</v>
       </c>
       <c r="J10" s="9">
         <v>10.3</v>
       </c>
       <c r="K10" s="9" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="L10" s="9" t="s">
         <v>8</v>
@@ -1886,17 +1892,17 @@
         <v>153</v>
       </c>
       <c r="H11" s="10" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I11" s="10">
         <f ca="1">ROUND(RAND()*(2-VALUE(I10))+VALUE(I10),2)</f>
-        <v>0.55000000000000004</v>
+        <v>1.92</v>
       </c>
       <c r="J11" s="10">
         <v>25.4</v>
       </c>
       <c r="K11" s="10" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="L11" s="10" t="s">
         <v>68</v>
@@ -1943,11 +1949,11 @@
         <v>89</v>
       </c>
       <c r="H12" s="9" t="s">
-        <v>253</v>
+        <v>224</v>
       </c>
       <c r="I12" s="9">
         <f ca="1">ROUND(RAND()*(0.64-0.3)+0.3, 2)</f>
-        <v>0.61</v>
+        <v>0.36</v>
       </c>
       <c r="J12" s="9">
         <v>1</v>
@@ -2000,11 +2006,11 @@
         <v>89</v>
       </c>
       <c r="H13" t="s">
-        <v>254</v>
+        <v>225</v>
       </c>
       <c r="I13">
         <f ca="1">ROUND(RAND()*(1-VALUE(I12))+VALUE(I12),2)</f>
-        <v>0.79</v>
+        <v>0.64</v>
       </c>
       <c r="J13">
         <v>4.5</v>
@@ -2056,7 +2062,7 @@
       </c>
       <c r="I14" s="10">
         <f ca="1">ROUND(RAND()*(2-VALUE(I13))+VALUE(I13),2)</f>
-        <v>0.87</v>
+        <v>1.72</v>
       </c>
       <c r="J14" s="10">
         <v>39.200000000000003</v>
@@ -2106,21 +2112,21 @@
         <v>68</v>
       </c>
       <c r="G15" s="9" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H15" t="s">
-        <v>197</v>
+        <v>234</v>
       </c>
       <c r="I15">
         <f ca="1">ROUND(RAND()*(0.6-0.3)+0.3, 2)</f>
-        <v>0.54</v>
+        <v>0.44</v>
       </c>
       <c r="J15" s="9">
         <f ca="1">ROUND(RAND()*(10 -1)+1,2)</f>
-        <v>8.61</v>
+        <v>6.14</v>
       </c>
       <c r="K15" s="9" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="L15" s="9" t="s">
         <v>32</v>
@@ -2164,21 +2170,21 @@
         <v>74</v>
       </c>
       <c r="G16" s="10" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H16" t="s">
-        <v>198</v>
+        <v>235</v>
       </c>
       <c r="I16" s="10">
         <f ca="1">ROUND(RAND()*(2-1)+1,2)</f>
-        <v>1.43</v>
+        <v>1.93</v>
       </c>
       <c r="J16" s="10">
         <f ca="1">ROUND(RAND()*(100-VALUE(J15))+VALUE(J15),2)</f>
-        <v>13.44</v>
+        <v>80.17</v>
       </c>
       <c r="K16" s="9" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="L16" s="10" t="s">
         <v>68</v>
@@ -2225,18 +2231,18 @@
         <v>90</v>
       </c>
       <c r="H17" t="s">
-        <v>201</v>
+        <v>236</v>
       </c>
       <c r="I17" s="9">
         <f ca="1">ROUND(RAND()*(0.6-0.3)+0.3, 2)</f>
-        <v>0.53</v>
+        <v>0.38</v>
       </c>
       <c r="J17" s="9">
         <f ca="1">ROUND(RAND()*(10 -1)+1,2)</f>
-        <v>6.78</v>
+        <v>1.45</v>
       </c>
       <c r="K17" s="9" t="s">
-        <v>203</v>
+        <v>193</v>
       </c>
       <c r="L17" s="9" t="s">
         <v>28</v>
@@ -2283,18 +2289,18 @@
         <v>90</v>
       </c>
       <c r="H18" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
       <c r="I18" s="10">
         <f ca="1">ROUND(RAND()*(2-1)+1,2)</f>
-        <v>1.1599999999999999</v>
+        <v>1.89</v>
       </c>
       <c r="J18" s="10">
         <f ca="1">ROUND(RAND()*(100-VALUE(J17))+VALUE(J17),2)</f>
-        <v>57.79</v>
+        <v>54.1</v>
       </c>
       <c r="K18" s="9" t="s">
-        <v>204</v>
+        <v>194</v>
       </c>
       <c r="L18" s="10" t="s">
         <v>68</v>
@@ -2341,18 +2347,18 @@
         <v>91</v>
       </c>
       <c r="H19" t="s">
-        <v>206</v>
+        <v>196</v>
       </c>
       <c r="I19" s="9">
         <f ca="1">ROUND(RAND()*(1-0.3)+0.3, 2)</f>
-        <v>0.32</v>
+        <v>0.83</v>
       </c>
       <c r="J19" s="9">
         <f ca="1">ROUND(RAND()*(10 -1)+1,2)</f>
-        <v>5.46</v>
+        <v>6.7</v>
       </c>
       <c r="K19" s="9" t="s">
-        <v>68</v>
+        <v>258</v>
       </c>
       <c r="L19" s="9" t="s">
         <v>29</v>
@@ -2396,21 +2402,21 @@
         <v>74</v>
       </c>
       <c r="G20" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H20" t="s">
-        <v>207</v>
+        <v>237</v>
       </c>
       <c r="I20" s="10">
         <f ca="1">ROUND(RAND()*(2-0.8)+0.8,2)</f>
-        <v>1.34</v>
+        <v>0.95</v>
       </c>
       <c r="J20" s="10">
         <f ca="1">ROUND(RAND()*(100-VALUE(J19))+VALUE(J19),2)</f>
-        <v>47.28</v>
+        <v>37.770000000000003</v>
       </c>
       <c r="K20" s="9" t="s">
-        <v>68</v>
+        <v>257</v>
       </c>
       <c r="L20" t="s">
         <v>30</v>
@@ -2449,21 +2455,21 @@
         <v>74</v>
       </c>
       <c r="G21" s="10" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="H21" s="10" t="s">
-        <v>208</v>
+        <v>197</v>
       </c>
       <c r="I21" s="10">
         <f ca="1">ROUND(RAND()*(2-VALUE(I20))+VALUE(I20),2)</f>
-        <v>1.38</v>
+        <v>1.76</v>
       </c>
       <c r="J21" s="10">
         <f ca="1">ROUND(RAND()*(200-VALUE(J20))+VALUE(J20),2)</f>
-        <v>58.64</v>
+        <v>79.16</v>
       </c>
       <c r="K21" s="9" t="s">
-        <v>68</v>
+        <v>257</v>
       </c>
       <c r="L21" s="10" t="s">
         <v>68</v>
@@ -2510,18 +2516,18 @@
         <v>92</v>
       </c>
       <c r="H22" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I22" s="9">
         <f ca="1">ROUND(RAND()*(0.5-0.3)+0.3, 2)</f>
-        <v>0.42</v>
+        <v>0.34</v>
       </c>
       <c r="J22" s="9">
         <f ca="1">ROUND(RAND()*(10 -1)+1,2)</f>
-        <v>4.72</v>
+        <v>1.48</v>
       </c>
       <c r="K22" s="9" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="L22" s="9" t="s">
         <v>47</v>
@@ -2568,18 +2574,18 @@
         <v>92</v>
       </c>
       <c r="H23" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I23" s="10">
         <f ca="1">ROUND(RAND()*(1-VALUE(I22))+VALUE(I22),2)</f>
-        <v>0.99</v>
+        <v>0.59</v>
       </c>
       <c r="J23" s="10">
         <f ca="1">ROUND(RAND()*(100-VALUE(J22))+VALUE(J22),2)</f>
-        <v>38.659999999999997</v>
+        <v>45.73</v>
       </c>
       <c r="K23" s="9" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="L23" s="10" t="s">
         <v>68</v>
@@ -2623,21 +2629,21 @@
         <v>68</v>
       </c>
       <c r="G24" s="9" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H24" t="s">
-        <v>209</v>
+        <v>238</v>
       </c>
       <c r="I24" s="9">
         <f ca="1">ROUND(RAND()*(0.5-0.3)+0.3, 2)</f>
-        <v>0.34</v>
+        <v>0.5</v>
       </c>
       <c r="J24" s="9">
         <f ca="1">ROUND(RAND()*(10 -1)+1,2)</f>
-        <v>8</v>
+        <v>6.8</v>
       </c>
       <c r="K24" s="9" t="s">
-        <v>210</v>
+        <v>198</v>
       </c>
       <c r="L24" s="9" t="s">
         <v>48</v>
@@ -2681,21 +2687,21 @@
         <v>72</v>
       </c>
       <c r="G25" s="10" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
       <c r="H25" t="s">
-        <v>211</v>
+        <v>239</v>
       </c>
       <c r="I25" s="10">
         <f ca="1">ROUND(RAND()*(1-VALUE(I24))+VALUE(I24),2)</f>
-        <v>0.43</v>
+        <v>0.94</v>
       </c>
       <c r="J25" s="10">
         <f ca="1">ROUND(RAND()*(100-VALUE(J24))+VALUE(J24),2)</f>
-        <v>74.22</v>
+        <v>94.06</v>
       </c>
       <c r="K25" s="9" t="s">
-        <v>212</v>
+        <v>199</v>
       </c>
       <c r="L25" s="10" t="s">
         <v>68</v>
@@ -2739,21 +2745,21 @@
         <v>72</v>
       </c>
       <c r="G26" s="9" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="H26" t="s">
-        <v>255</v>
+        <v>226</v>
       </c>
       <c r="I26" s="9">
         <f ca="1">ROUND(RAND()*(0.6-0.3)+0.3, 2)</f>
-        <v>0.52</v>
+        <v>0.44</v>
       </c>
       <c r="J26" s="9">
         <f ca="1">ROUND(RAND()*(10 -1)+1,2)</f>
-        <v>5.0599999999999996</v>
+        <v>3.96</v>
       </c>
       <c r="K26" s="9" t="s">
-        <v>213</v>
+        <v>200</v>
       </c>
       <c r="L26" s="9" t="s">
         <v>33</v>
@@ -2797,21 +2803,21 @@
         <v>72</v>
       </c>
       <c r="G27" s="10" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H27" t="s">
-        <v>214</v>
+        <v>240</v>
       </c>
       <c r="I27" s="10">
         <f ca="1">ROUND(RAND()*(1.2-VALUE(I26))+VALUE(I26),2)</f>
-        <v>0.96</v>
+        <v>0.72</v>
       </c>
       <c r="J27" s="10">
         <f ca="1">ROUND(RAND()*(100-VALUE(J26))+VALUE(J26),2)</f>
-        <v>46.95</v>
+        <v>77.23</v>
       </c>
       <c r="K27" s="9" t="s">
-        <v>215</v>
+        <v>201</v>
       </c>
       <c r="L27" s="10" t="s">
         <v>68</v>
@@ -2855,21 +2861,21 @@
         <v>72</v>
       </c>
       <c r="G28" s="9" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H28" t="s">
-        <v>217</v>
+        <v>241</v>
       </c>
       <c r="I28" s="9">
         <f ca="1">ROUND(RAND()*(0.6-0.3)+0.3, 2)</f>
-        <v>0.51</v>
+        <v>0.45</v>
       </c>
       <c r="J28" s="9">
         <f ca="1">ROUND(RAND()*(10 -1)+1,2)</f>
-        <v>2.86</v>
+        <v>6.35</v>
       </c>
       <c r="K28" s="9" t="s">
-        <v>216</v>
+        <v>202</v>
       </c>
       <c r="L28" s="9" t="s">
         <v>35</v>
@@ -2913,21 +2919,21 @@
         <v>72</v>
       </c>
       <c r="G29" s="10" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H29" t="s">
-        <v>218</v>
+        <v>203</v>
       </c>
       <c r="I29" s="10">
         <f ca="1">ROUND(RAND()*(0.9-VALUE(I28))+VALUE(I28),2)</f>
-        <v>0.65</v>
+        <v>0.85</v>
       </c>
       <c r="J29" s="10">
         <f ca="1">ROUND(RAND()*(100-VALUE(J28))+VALUE(J28),2)</f>
-        <v>30.46</v>
+        <v>39.409999999999997</v>
       </c>
       <c r="K29" s="10" t="s">
-        <v>219</v>
+        <v>204</v>
       </c>
       <c r="L29" s="10" t="s">
         <v>68</v>
@@ -2974,18 +2980,18 @@
         <v>93</v>
       </c>
       <c r="H30" t="s">
-        <v>220</v>
+        <v>242</v>
       </c>
       <c r="I30" s="9">
         <f ca="1">ROUND(RAND()*(0.8-0.3)+0.3, 2)</f>
-        <v>0.8</v>
+        <v>0.43</v>
       </c>
       <c r="J30" s="9">
         <f ca="1">ROUND(RAND()*(10 -1)+1,2)</f>
-        <v>4.76</v>
+        <v>7.76</v>
       </c>
       <c r="K30" s="9" t="s">
-        <v>222</v>
+        <v>205</v>
       </c>
       <c r="L30" s="9" t="s">
         <v>22</v>
@@ -3032,18 +3038,18 @@
         <v>93</v>
       </c>
       <c r="H31" t="s">
-        <v>221</v>
+        <v>243</v>
       </c>
       <c r="I31" s="10">
         <f ca="1">ROUND(RAND()*(2-VALUE(I30))+VALUE(I30),2)</f>
-        <v>1.37</v>
+        <v>1.81</v>
       </c>
       <c r="J31" s="10">
         <f ca="1">ROUND(RAND()*(100-VALUE(J30))+VALUE(J30),2)</f>
-        <v>10.44</v>
+        <v>77.63</v>
       </c>
       <c r="K31" s="10" t="s">
-        <v>222</v>
+        <v>205</v>
       </c>
       <c r="L31" s="10" t="s">
         <v>68</v>
@@ -3090,18 +3096,18 @@
         <v>94</v>
       </c>
       <c r="H32" t="s">
-        <v>223</v>
+        <v>206</v>
       </c>
       <c r="I32" s="9">
         <f ca="1">ROUND(RAND()*(0.5-0.3)+0.3, 2)</f>
-        <v>0.33</v>
+        <v>0.41</v>
       </c>
       <c r="J32" s="9">
         <f ca="1">ROUND(RAND()*(10 -1)+1,2)</f>
-        <v>7.13</v>
+        <v>2.48</v>
       </c>
       <c r="K32" s="9" t="s">
-        <v>224</v>
+        <v>207</v>
       </c>
       <c r="L32" s="9" t="s">
         <v>39</v>
@@ -3148,18 +3154,18 @@
         <v>95</v>
       </c>
       <c r="H33" t="s">
-        <v>225</v>
+        <v>208</v>
       </c>
       <c r="I33" s="10">
         <f ca="1">ROUND(RAND()*(0.8-VALUE(I32))+VALUE(I32),2)</f>
-        <v>0.51</v>
+        <v>0.44</v>
       </c>
       <c r="J33" s="10">
         <f ca="1">ROUND(RAND()*(100-VALUE(J32))+VALUE(J32),2)</f>
-        <v>12.54</v>
+        <v>68.22</v>
       </c>
       <c r="K33" t="s">
-        <v>228</v>
+        <v>210</v>
       </c>
       <c r="L33" t="s">
         <v>38</v>
@@ -3201,18 +3207,18 @@
         <v>95</v>
       </c>
       <c r="H34" t="s">
-        <v>227</v>
+        <v>244</v>
       </c>
       <c r="I34" s="10">
         <f ca="1">ROUND(RAND()*(2-VALUE(I33))+VALUE(I33),2)</f>
-        <v>1.41</v>
+        <v>1.82</v>
       </c>
       <c r="J34" s="10">
         <f ca="1">ROUND(RAND()*(200-VALUE(J33))+VALUE(J33),2)</f>
-        <v>78.099999999999994</v>
+        <v>199.8</v>
       </c>
       <c r="K34" s="10" t="s">
-        <v>228</v>
+        <v>210</v>
       </c>
       <c r="L34" s="10" t="s">
         <v>68</v>
@@ -3259,18 +3265,18 @@
         <v>96</v>
       </c>
       <c r="H35" t="s">
-        <v>229</v>
+        <v>245</v>
       </c>
       <c r="I35" s="9">
         <f ca="1">ROUND(RAND()*(1-0.3)+0.3, 2)</f>
-        <v>0.86</v>
+        <v>0.4</v>
       </c>
       <c r="J35" s="9">
         <f ca="1">ROUND(RAND()*(10 -1)+1,2)</f>
-        <v>3.53</v>
+        <v>3.72</v>
       </c>
       <c r="K35" s="9" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="L35" s="9" t="s">
         <v>41</v>
@@ -3317,18 +3323,18 @@
         <v>96</v>
       </c>
       <c r="H36" t="s">
-        <v>230</v>
+        <v>211</v>
       </c>
       <c r="I36" s="10">
         <f ca="1">ROUND(RAND()*(1-VALUE(I35))+VALUE(I35),2)</f>
-        <v>0.89</v>
+        <v>0.77</v>
       </c>
       <c r="J36" s="10">
         <f ca="1">ROUND(RAND()*(100-VALUE(J35))+VALUE(J35),2)</f>
-        <v>87.96</v>
+        <v>4.8899999999999997</v>
       </c>
       <c r="K36" s="10" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="L36" s="10" t="s">
         <v>68</v>
@@ -3372,21 +3378,21 @@
         <v>68</v>
       </c>
       <c r="G37" s="9" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H37" t="s">
-        <v>231</v>
+        <v>246</v>
       </c>
       <c r="I37" s="9">
         <f ca="1">ROUND(RAND()*(0.8-0.3)+0.3, 2)</f>
-        <v>0.63</v>
+        <v>0.44</v>
       </c>
       <c r="J37" s="9">
         <f ca="1">ROUND(RAND()*(10 -1)+1,2)</f>
-        <v>7.45</v>
+        <v>1.84</v>
       </c>
       <c r="K37" s="9" t="s">
-        <v>233</v>
+        <v>213</v>
       </c>
       <c r="L37" s="9" t="s">
         <v>42</v>
@@ -3430,21 +3436,21 @@
         <v>77</v>
       </c>
       <c r="G38" s="10" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H38" t="s">
-        <v>232</v>
+        <v>212</v>
       </c>
       <c r="I38" s="10">
         <f ca="1">ROUND(RAND()*(1.4-VALUE(I37))+VALUE(I37),2)</f>
-        <v>1.08</v>
+        <v>0.46</v>
       </c>
       <c r="J38" s="10">
         <f ca="1">ROUND(RAND()*(100-VALUE(J37))+VALUE(J37),2)</f>
-        <v>32.909999999999997</v>
+        <v>49.19</v>
       </c>
       <c r="K38" s="10" t="s">
-        <v>234</v>
+        <v>214</v>
       </c>
       <c r="L38" s="10" t="s">
         <v>68</v>
@@ -3488,20 +3494,20 @@
         <v>68</v>
       </c>
       <c r="G39" s="9" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="H39" t="s">
-        <v>235</v>
+        <v>215</v>
       </c>
       <c r="I39" s="9">
         <v>0.6</v>
       </c>
       <c r="J39" s="9">
         <f ca="1">ROUND(RAND()*(10 -1)+1,2)</f>
-        <v>2.35</v>
+        <v>6.17</v>
       </c>
       <c r="K39" s="9" t="s">
-        <v>236</v>
+        <v>216</v>
       </c>
       <c r="L39" s="9" t="s">
         <v>45</v>
@@ -3545,21 +3551,21 @@
         <v>72</v>
       </c>
       <c r="G40" s="10" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H40" t="s">
-        <v>237</v>
+        <v>247</v>
       </c>
       <c r="I40" s="10">
         <f ca="1">ROUND(RAND()*(1.2-VALUE(I39))+VALUE(I39),2)</f>
-        <v>0.94</v>
+        <v>0.97</v>
       </c>
       <c r="J40" s="10">
         <f ca="1">ROUND(RAND()*(100-VALUE(J39))+VALUE(J39),2)</f>
-        <v>4.95</v>
+        <v>30.35</v>
       </c>
       <c r="K40" s="10" t="s">
-        <v>238</v>
+        <v>217</v>
       </c>
       <c r="L40" s="10" t="s">
         <v>68</v>
@@ -3606,18 +3612,18 @@
         <v>97</v>
       </c>
       <c r="H41" t="s">
-        <v>239</v>
+        <v>248</v>
       </c>
       <c r="I41" s="11">
         <f ca="1">ROUND(RAND()*(0.5-0.3)+0.3, 2)</f>
-        <v>0.3</v>
+        <v>0.35</v>
       </c>
       <c r="J41" s="9">
         <f ca="1">ROUND(RAND()*(10 -1)+1,2)</f>
-        <v>6.77</v>
+        <v>2.34</v>
       </c>
       <c r="K41" s="11" t="s">
-        <v>210</v>
+        <v>198</v>
       </c>
       <c r="L41" s="11" t="s">
         <v>68</v>
@@ -3664,18 +3670,18 @@
         <v>98</v>
       </c>
       <c r="H42" t="s">
-        <v>240</v>
+        <v>249</v>
       </c>
       <c r="I42" s="11">
         <f ca="1">ROUND(RAND()*(0.5-0.3)+0.3, 2)</f>
-        <v>0.43</v>
+        <v>0.36</v>
       </c>
       <c r="J42" s="9">
         <f ca="1">ROUND(RAND()*(10 -1)+1,2)</f>
-        <v>2.46</v>
+        <v>9.77</v>
       </c>
       <c r="K42" s="11" t="s">
-        <v>248</v>
+        <v>219</v>
       </c>
       <c r="L42" s="11" t="s">
         <v>68</v>
@@ -3722,18 +3728,18 @@
         <v>99</v>
       </c>
       <c r="H43" t="s">
-        <v>241</v>
+        <v>250</v>
       </c>
       <c r="I43" s="9">
         <f ca="1">ROUND(RAND()*(2-1)+1, 2)</f>
-        <v>1.7</v>
+        <v>1.24</v>
       </c>
       <c r="J43" s="9">
         <f ca="1">ROUND(RAND()*(10 -1)+1,2)</f>
-        <v>5.21</v>
+        <v>5.87</v>
       </c>
       <c r="K43" s="9" t="s">
-        <v>249</v>
+        <v>220</v>
       </c>
       <c r="L43" s="9" t="s">
         <v>19</v>
@@ -3777,21 +3783,21 @@
         <v>74</v>
       </c>
       <c r="G44" s="10" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="H44" t="s">
-        <v>242</v>
+        <v>251</v>
       </c>
       <c r="I44" s="10">
         <f ca="1">ROUND(RAND()*(2-VALUE(I43))+VALUE(I43),2)</f>
-        <v>1.8</v>
+        <v>1.46</v>
       </c>
       <c r="J44" s="10">
         <f ca="1">ROUND(RAND()*(100-VALUE(J43))+VALUE(J43),2)</f>
-        <v>41.95</v>
+        <v>47.02</v>
       </c>
       <c r="K44" s="10" t="s">
-        <v>250</v>
+        <v>221</v>
       </c>
       <c r="L44" s="10" t="s">
         <v>68</v>
@@ -3835,21 +3841,21 @@
         <v>82</v>
       </c>
       <c r="G45" s="11" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H45" t="s">
-        <v>243</v>
+        <v>252</v>
       </c>
       <c r="I45" s="9">
         <f ca="1">ROUND(RAND()*(2-1)+1, 2)</f>
-        <v>1.69</v>
+        <v>1.53</v>
       </c>
       <c r="J45" s="9">
         <f t="shared" ref="J45:J50" ca="1" si="0">ROUND(RAND()*(10 -1)+1,2)</f>
-        <v>5.71</v>
+        <v>5.43</v>
       </c>
       <c r="K45" s="11" t="s">
-        <v>226</v>
+        <v>209</v>
       </c>
       <c r="L45" s="11" t="s">
         <v>68</v>
@@ -3896,18 +3902,18 @@
         <v>100</v>
       </c>
       <c r="H46" t="s">
-        <v>244</v>
+        <v>253</v>
       </c>
       <c r="I46" s="9">
         <f ca="1">ROUND(RAND()*(2-1)+1, 2)</f>
-        <v>1.72</v>
+        <v>1.04</v>
       </c>
       <c r="J46" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>6.27</v>
+        <v>3.98</v>
       </c>
       <c r="K46" s="11" t="s">
-        <v>251</v>
+        <v>222</v>
       </c>
       <c r="L46" s="11" t="s">
         <v>68</v>
@@ -3951,21 +3957,21 @@
         <v>87</v>
       </c>
       <c r="G47" s="11" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="H47" t="s">
-        <v>245</v>
+        <v>254</v>
       </c>
       <c r="I47" s="9">
         <f ca="1">ROUND(RAND()*(2-1)+1, 2)</f>
-        <v>1.57</v>
+        <v>1.17</v>
       </c>
       <c r="J47" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>4.92</v>
+        <v>4.1900000000000004</v>
       </c>
       <c r="K47" s="11" t="s">
-        <v>252</v>
+        <v>223</v>
       </c>
       <c r="L47" s="11" t="s">
         <v>68</v>
@@ -4012,18 +4018,18 @@
         <v>101</v>
       </c>
       <c r="H48" s="11" t="s">
-        <v>183</v>
+        <v>255</v>
       </c>
       <c r="I48" s="9">
         <f ca="1">ROUND(RAND()*(2-1)+1, 2)</f>
-        <v>1.08</v>
+        <v>1.98</v>
       </c>
       <c r="J48" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>7.7</v>
+        <v>2.5299999999999998</v>
       </c>
       <c r="K48" s="11" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="L48" s="11" t="s">
         <v>68</v>
@@ -4067,21 +4073,21 @@
         <v>72</v>
       </c>
       <c r="G49" s="11" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="H49" t="s">
-        <v>246</v>
+        <v>256</v>
       </c>
       <c r="I49" s="11">
         <f ca="1">ROUND(RAND()*(1.4-1)+1, 2)</f>
-        <v>1.03</v>
+        <v>1.23</v>
       </c>
       <c r="J49" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>3.2</v>
+        <v>5.53</v>
       </c>
       <c r="K49" s="11" t="s">
-        <v>247</v>
+        <v>218</v>
       </c>
       <c r="L49" s="11" t="s">
         <v>68</v>
@@ -4125,21 +4131,21 @@
         <v>68</v>
       </c>
       <c r="G50" s="10" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="H50" s="10" t="s">
-        <v>256</v>
+        <v>227</v>
       </c>
       <c r="I50" s="10">
         <f ca="1">ROUND(RAND()*(0.5-0.3)+0.3, 2)</f>
-        <v>0.31</v>
+        <v>0.45</v>
       </c>
       <c r="J50" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>3.19</v>
+        <v>6.3</v>
       </c>
       <c r="K50" s="10" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="L50" s="10" t="s">
         <v>68</v>

</xml_diff>

<commit_message>
removed mesh and anim data from data tables
</commit_message>
<xml_diff>
--- a/Content/_Data/Pokemon/pokemon-data.xlsx
+++ b/Content/_Data/Pokemon/pokemon-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Unreal\PokemonRemake\Content\_Data\Pokemon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCD65155-4AC2-4BE3-99D8-8FC1CB489060}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{299745D1-0DC3-434E-A81F-4400816E0ABD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="253">
   <si>
     <t>Alien</t>
   </si>
@@ -213,15 +213,6 @@
     <t>EvolvesTo</t>
   </si>
   <si>
-    <t>PokemonMesh</t>
-  </si>
-  <si>
-    <t>AnimBP</t>
-  </si>
-  <si>
-    <t>AttackAnim</t>
-  </si>
-  <si>
     <t>BaseHP</t>
   </si>
   <si>
@@ -232,15 +223,6 @@
   </si>
   <si>
     <t>BaseSpeed</t>
-  </si>
-  <si>
-    <t>DeathAnim</t>
-  </si>
-  <si>
-    <t>HitAnim</t>
-  </si>
-  <si>
-    <t>DodgeAnim</t>
   </si>
   <si>
     <t>None</t>
@@ -1259,10 +1241,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55723188-F4D3-4EF4-AEA8-7A04D3578F8F}">
-  <dimension ref="A1:V50"/>
+  <dimension ref="A1:P50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="Q1" sqref="Q1:V1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1274,13 +1256,9 @@
     <col min="9" max="9" width="14" customWidth="1"/>
     <col min="11" max="11" width="27.42578125" customWidth="1"/>
     <col min="12" max="12" width="22" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.7109375" customWidth="1"/>
-    <col min="19" max="19" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="13.42578125" customWidth="1"/>
-    <col min="22" max="22" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>49</v>
       </c>
@@ -1291,7 +1269,7 @@
         <v>51</v>
       </c>
       <c r="D1" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="E1" t="s">
         <v>52</v>
@@ -1309,46 +1287,28 @@
         <v>56</v>
       </c>
       <c r="J1" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="K1" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="L1" t="s">
         <v>57</v>
       </c>
       <c r="M1" t="s">
+        <v>58</v>
+      </c>
+      <c r="N1" t="s">
+        <v>59</v>
+      </c>
+      <c r="O1" t="s">
+        <v>60</v>
+      </c>
+      <c r="P1" t="s">
         <v>61</v>
       </c>
-      <c r="N1" t="s">
-        <v>62</v>
-      </c>
-      <c r="O1" t="s">
-        <v>63</v>
-      </c>
-      <c r="P1" t="s">
-        <v>64</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>58</v>
-      </c>
-      <c r="R1" t="s">
-        <v>59</v>
-      </c>
-      <c r="S1" t="s">
-        <v>60</v>
-      </c>
-      <c r="T1" t="s">
-        <v>65</v>
-      </c>
-      <c r="U1" t="s">
-        <v>66</v>
-      </c>
-      <c r="V1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>0</v>
       </c>
@@ -1359,30 +1319,30 @@
         <v>0</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="H2" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="I2" s="9">
         <f ca="1">ROUND(RAND()*(0.6-0.3)+0.3, 2)</f>
-        <v>0.56999999999999995</v>
+        <v>0.43</v>
       </c>
       <c r="J2" s="9">
         <f ca="1">ROUND(RAND()*(10 -1)+1,2)</f>
-        <v>6.93</v>
+        <v>1.92</v>
       </c>
       <c r="K2" s="9" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="L2" s="9" t="s">
         <v>17</v>
@@ -1399,14 +1359,8 @@
       <c r="P2" s="9">
         <v>100</v>
       </c>
-      <c r="Q2" s="9"/>
-      <c r="R2" s="9"/>
-      <c r="S2" s="9"/>
-      <c r="T2" s="9"/>
-      <c r="U2" s="9"/>
-      <c r="V2" s="2"/>
-    </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>17</v>
       </c>
@@ -1417,33 +1371,33 @@
         <v>17</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="H3" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="I3" s="10">
         <f ca="1">ROUND(RAND()*(2-VALUE(I2))+VALUE(I2),2)</f>
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="J3" s="10">
         <f ca="1">ROUND(RAND()*(100-VALUE(J2))+VALUE(J2),2)</f>
-        <v>52.04</v>
+        <v>33.42</v>
       </c>
       <c r="K3" s="9" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="L3" s="10" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="M3" s="10">
         <v>80</v>
@@ -1457,14 +1411,8 @@
       <c r="P3" s="10">
         <v>120</v>
       </c>
-      <c r="Q3" s="10"/>
-      <c r="R3" s="10"/>
-      <c r="S3" s="10"/>
-      <c r="T3" s="10"/>
-      <c r="U3" s="10"/>
-      <c r="V3" s="4"/>
-    </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>1</v>
       </c>
@@ -1475,30 +1423,30 @@
         <v>1</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="H4" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="I4" s="9">
         <f ca="1">ROUND(RAND()*(0.6-0.3)+0.3, 2)</f>
-        <v>0.49</v>
+        <v>0.54</v>
       </c>
       <c r="J4" s="9">
         <f ca="1">ROUND(RAND()*(10 -1)+1,2)</f>
-        <v>1.94</v>
+        <v>9.68</v>
       </c>
       <c r="K4" s="9" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="L4" s="9" t="s">
         <v>18</v>
@@ -1515,14 +1463,8 @@
       <c r="P4" s="9">
         <v>70</v>
       </c>
-      <c r="Q4" s="9"/>
-      <c r="R4" s="9"/>
-      <c r="S4" s="9"/>
-      <c r="T4" s="9"/>
-      <c r="U4" s="9"/>
-      <c r="V4" s="2"/>
-    </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>18</v>
       </c>
@@ -1533,33 +1475,33 @@
         <v>18</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="H5" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="I5" s="10">
         <f ca="1">ROUND(RAND()*(2-VALUE(I4))+VALUE(I4),2)</f>
-        <v>1.37</v>
+        <v>1.47</v>
       </c>
       <c r="J5" s="10">
         <f ca="1">ROUND(RAND()*(100-VALUE(J4))+VALUE(J4),2)</f>
-        <v>87.34</v>
+        <v>21.6</v>
       </c>
       <c r="K5" s="9" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="L5" s="10" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="M5" s="10">
         <v>40</v>
@@ -1573,14 +1515,8 @@
       <c r="P5" s="10">
         <v>100</v>
       </c>
-      <c r="Q5" s="10"/>
-      <c r="R5" s="10"/>
-      <c r="S5" s="10"/>
-      <c r="T5" s="10"/>
-      <c r="U5" s="10"/>
-      <c r="V5" s="4"/>
-    </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>2</v>
       </c>
@@ -1594,27 +1530,27 @@
         <v>2</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="H6" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="I6" s="9">
         <f ca="1">ROUND(RAND()*(0.8-0.3)+0.3, 2)</f>
-        <v>0.66</v>
+        <v>0.69</v>
       </c>
       <c r="J6" s="9">
         <f ca="1">ROUND(RAND()*(10 -1)+1,2)</f>
-        <v>4.18</v>
+        <v>3.9</v>
       </c>
       <c r="K6" s="9" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="L6" s="9" t="s">
         <v>21</v>
@@ -1631,14 +1567,8 @@
       <c r="P6" s="9">
         <v>40</v>
       </c>
-      <c r="Q6" s="9"/>
-      <c r="R6" s="9"/>
-      <c r="S6" s="9"/>
-      <c r="T6" s="9"/>
-      <c r="U6" s="9"/>
-      <c r="V6" s="2"/>
-    </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>21</v>
       </c>
@@ -1649,33 +1579,33 @@
         <v>21</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="G7" s="10" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="H7" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="I7" s="10">
         <f ca="1">ROUND(RAND()*(2-VALUE(I6))+VALUE(I6),2)</f>
-        <v>1.85</v>
+        <v>1.46</v>
       </c>
       <c r="J7" s="10">
         <f ca="1">ROUND(RAND()*(100-VALUE(J6))+VALUE(J6),2)</f>
-        <v>67.400000000000006</v>
+        <v>88.97</v>
       </c>
       <c r="K7" s="9" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="L7" s="10" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="M7" s="10">
         <v>90</v>
@@ -1689,14 +1619,8 @@
       <c r="P7" s="10">
         <v>60</v>
       </c>
-      <c r="Q7" s="10"/>
-      <c r="R7" s="10"/>
-      <c r="S7" s="10"/>
-      <c r="T7" s="10"/>
-      <c r="U7" s="10"/>
-      <c r="V7" s="4"/>
-    </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>6</v>
       </c>
@@ -1707,30 +1631,30 @@
         <v>6</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="H8" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="I8" s="9">
         <f ca="1">ROUND(RAND()*(0.5-0.3)+0.3, 2)</f>
-        <v>0.4</v>
+        <v>0.49</v>
       </c>
       <c r="J8" s="9">
         <f ca="1">ROUND(RAND()*(10 -1)+1,2)</f>
-        <v>8.6</v>
+        <v>7.02</v>
       </c>
       <c r="K8" s="9" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="L8" s="9" t="s">
         <v>24</v>
@@ -1747,14 +1671,8 @@
       <c r="P8" s="9">
         <v>50</v>
       </c>
-      <c r="Q8" s="9"/>
-      <c r="R8" s="9"/>
-      <c r="S8" s="9"/>
-      <c r="T8" s="9"/>
-      <c r="U8" s="9"/>
-      <c r="V8" s="2"/>
-    </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
         <v>24</v>
       </c>
@@ -1765,33 +1683,33 @@
         <v>24</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="G9" s="10" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="H9" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="I9" s="10">
         <f ca="1">ROUND(RAND()*(2-VALUE(I8))+VALUE(I8),2)</f>
-        <v>0.7</v>
+        <v>1.49</v>
       </c>
       <c r="J9" s="10">
         <f ca="1">ROUND(RAND()*(100-VALUE(J8))+VALUE(J8),2)</f>
-        <v>17.36</v>
+        <v>91.23</v>
       </c>
       <c r="K9" s="9" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="L9" s="10" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="M9" s="10">
         <v>80</v>
@@ -1805,14 +1723,8 @@
       <c r="P9" s="10">
         <v>80</v>
       </c>
-      <c r="Q9" s="10"/>
-      <c r="R9" s="10"/>
-      <c r="S9" s="10"/>
-      <c r="T9" s="10"/>
-      <c r="U9" s="10"/>
-      <c r="V9" s="4"/>
-    </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>7</v>
       </c>
@@ -1823,29 +1735,29 @@
         <v>7</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="H10" s="9" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="I10" s="9">
         <f ca="1">ROUND(RAND()*(0.5-0.3)+0.3, 2)</f>
-        <v>0.43</v>
+        <v>0.44</v>
       </c>
       <c r="J10" s="9">
         <v>10.3</v>
       </c>
       <c r="K10" s="9" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="L10" s="9" t="s">
         <v>8</v>
@@ -1862,14 +1774,8 @@
       <c r="P10" s="9">
         <v>40</v>
       </c>
-      <c r="Q10" s="9"/>
-      <c r="R10" s="9"/>
-      <c r="S10" s="9"/>
-      <c r="T10" s="9"/>
-      <c r="U10" s="9"/>
-      <c r="V10" s="2"/>
-    </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
         <v>8</v>
       </c>
@@ -1880,32 +1786,32 @@
         <v>8</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="G11" s="10" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="H11" s="10" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="I11" s="10">
         <f ca="1">ROUND(RAND()*(2-VALUE(I10))+VALUE(I10),2)</f>
-        <v>1.92</v>
+        <v>1.52</v>
       </c>
       <c r="J11" s="10">
         <v>25.4</v>
       </c>
       <c r="K11" s="10" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="L11" s="10" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="M11" s="10">
         <v>80</v>
@@ -1919,14 +1825,8 @@
       <c r="P11" s="10">
         <v>50</v>
       </c>
-      <c r="Q11" s="10"/>
-      <c r="R11" s="10"/>
-      <c r="S11" s="10"/>
-      <c r="T11" s="10"/>
-      <c r="U11" s="10"/>
-      <c r="V11" s="4"/>
-    </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>10</v>
       </c>
@@ -1940,26 +1840,26 @@
         <v>10</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="H12" s="9" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="I12" s="9">
         <f ca="1">ROUND(RAND()*(0.64-0.3)+0.3, 2)</f>
-        <v>0.36</v>
+        <v>0.49</v>
       </c>
       <c r="J12" s="9">
         <v>1</v>
       </c>
       <c r="K12" s="9" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="L12" s="9" t="s">
         <v>9</v>
@@ -1976,14 +1876,8 @@
       <c r="P12" s="9">
         <v>15</v>
       </c>
-      <c r="Q12" s="9"/>
-      <c r="R12" s="9"/>
-      <c r="S12" s="9"/>
-      <c r="T12" s="9"/>
-      <c r="U12" s="9"/>
-      <c r="V12" s="2"/>
-    </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -1994,29 +1888,29 @@
         <v>9</v>
       </c>
       <c r="D13" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="E13" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="F13" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="G13" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="H13" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="I13">
         <f ca="1">ROUND(RAND()*(1-VALUE(I12))+VALUE(I12),2)</f>
-        <v>0.64</v>
+        <v>0.85</v>
       </c>
       <c r="J13">
         <v>4.5</v>
       </c>
       <c r="K13" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="L13" t="s">
         <v>27</v>
@@ -2033,9 +1927,8 @@
       <c r="P13">
         <v>35</v>
       </c>
-      <c r="V13" s="6"/>
-    </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
         <v>27</v>
       </c>
@@ -2046,32 +1939,32 @@
         <v>27</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="G14" s="10" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="H14" s="10" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="I14" s="10">
         <f ca="1">ROUND(RAND()*(2-VALUE(I13))+VALUE(I13),2)</f>
-        <v>1.72</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="J14" s="10">
         <v>39.200000000000003</v>
       </c>
       <c r="K14" s="10" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="L14" s="10" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="M14" s="10">
         <v>60</v>
@@ -2085,14 +1978,8 @@
       <c r="P14" s="10">
         <v>70</v>
       </c>
-      <c r="Q14" s="10"/>
-      <c r="R14" s="10"/>
-      <c r="S14" s="10"/>
-      <c r="T14" s="10"/>
-      <c r="U14" s="10"/>
-      <c r="V14" s="4"/>
-    </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>16</v>
       </c>
@@ -2103,30 +1990,30 @@
         <v>16</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="G15" s="9" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="H15" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="I15">
         <f ca="1">ROUND(RAND()*(0.6-0.3)+0.3, 2)</f>
-        <v>0.44</v>
+        <v>0.5</v>
       </c>
       <c r="J15" s="9">
         <f ca="1">ROUND(RAND()*(10 -1)+1,2)</f>
-        <v>6.14</v>
+        <v>6.84</v>
       </c>
       <c r="K15" s="9" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="L15" s="9" t="s">
         <v>32</v>
@@ -2143,14 +2030,8 @@
       <c r="P15" s="9">
         <v>40</v>
       </c>
-      <c r="Q15" s="9"/>
-      <c r="R15" s="9"/>
-      <c r="S15" s="9"/>
-      <c r="T15" s="9"/>
-      <c r="U15" s="9"/>
-      <c r="V15" s="2"/>
-    </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
         <v>32</v>
       </c>
@@ -2161,33 +2042,33 @@
         <v>32</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="F16" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="G16" s="10" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="H16" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="I16" s="10">
         <f ca="1">ROUND(RAND()*(2-1)+1,2)</f>
-        <v>1.93</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="J16" s="10">
         <f ca="1">ROUND(RAND()*(100-VALUE(J15))+VALUE(J15),2)</f>
-        <v>80.17</v>
+        <v>79.37</v>
       </c>
       <c r="K16" s="9" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="L16" s="10" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="M16" s="10">
         <v>80</v>
@@ -2201,14 +2082,8 @@
       <c r="P16" s="10">
         <v>70</v>
       </c>
-      <c r="Q16" s="10"/>
-      <c r="R16" s="10"/>
-      <c r="S16" s="10"/>
-      <c r="T16" s="10"/>
-      <c r="U16" s="10"/>
-      <c r="V16" s="4"/>
-    </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
         <v>11</v>
       </c>
@@ -2219,30 +2094,30 @@
         <v>11</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="F17" s="9" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="G17" s="9" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="H17" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="I17" s="9">
         <f ca="1">ROUND(RAND()*(0.6-0.3)+0.3, 2)</f>
-        <v>0.38</v>
+        <v>0.32</v>
       </c>
       <c r="J17" s="9">
         <f ca="1">ROUND(RAND()*(10 -1)+1,2)</f>
-        <v>1.45</v>
+        <v>5.97</v>
       </c>
       <c r="K17" s="9" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="L17" s="9" t="s">
         <v>28</v>
@@ -2259,14 +2134,8 @@
       <c r="P17" s="9">
         <v>95</v>
       </c>
-      <c r="Q17" s="9"/>
-      <c r="R17" s="9"/>
-      <c r="S17" s="9"/>
-      <c r="T17" s="9"/>
-      <c r="U17" s="9"/>
-      <c r="V17" s="2"/>
-    </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
         <v>28</v>
       </c>
@@ -2277,33 +2146,33 @@
         <v>28</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="F18" s="10" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="G18" s="10" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="H18" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="I18" s="10">
         <f ca="1">ROUND(RAND()*(2-1)+1,2)</f>
-        <v>1.89</v>
+        <v>1.21</v>
       </c>
       <c r="J18" s="10">
         <f ca="1">ROUND(RAND()*(100-VALUE(J17))+VALUE(J17),2)</f>
-        <v>54.1</v>
+        <v>12.59</v>
       </c>
       <c r="K18" s="9" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="L18" s="10" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="M18" s="10">
         <v>60</v>
@@ -2317,14 +2186,8 @@
       <c r="P18" s="10">
         <v>115</v>
       </c>
-      <c r="Q18" s="10"/>
-      <c r="R18" s="10"/>
-      <c r="S18" s="10"/>
-      <c r="T18" s="10"/>
-      <c r="U18" s="10"/>
-      <c r="V18" s="4"/>
-    </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
         <v>12</v>
       </c>
@@ -2335,30 +2198,30 @@
         <v>12</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="G19" s="9" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="H19" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="I19" s="9">
         <f ca="1">ROUND(RAND()*(1-0.3)+0.3, 2)</f>
-        <v>0.83</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="J19" s="9">
         <f ca="1">ROUND(RAND()*(10 -1)+1,2)</f>
-        <v>6.7</v>
+        <v>1.77</v>
       </c>
       <c r="K19" s="9" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="L19" s="9" t="s">
         <v>29</v>
@@ -2375,14 +2238,8 @@
       <c r="P19" s="9">
         <v>65</v>
       </c>
-      <c r="Q19" s="9"/>
-      <c r="R19" s="9"/>
-      <c r="S19" s="9"/>
-      <c r="T19" s="9"/>
-      <c r="U19" s="9"/>
-      <c r="V19" s="2"/>
-    </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>29</v>
       </c>
@@ -2393,30 +2250,30 @@
         <v>29</v>
       </c>
       <c r="D20" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="E20" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="F20" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="G20" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="H20" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="I20" s="10">
         <f ca="1">ROUND(RAND()*(2-0.8)+0.8,2)</f>
-        <v>0.95</v>
+        <v>1.37</v>
       </c>
       <c r="J20" s="10">
         <f ca="1">ROUND(RAND()*(100-VALUE(J19))+VALUE(J19),2)</f>
-        <v>37.770000000000003</v>
+        <v>15.19</v>
       </c>
       <c r="K20" s="9" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="L20" t="s">
         <v>30</v>
@@ -2433,9 +2290,8 @@
       <c r="P20">
         <v>75</v>
       </c>
-      <c r="V20" s="6"/>
-    </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="10" t="s">
         <v>30</v>
       </c>
@@ -2446,33 +2302,33 @@
         <v>30</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="E21" s="10" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="F21" s="10" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="G21" s="10" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="H21" s="10" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="I21" s="10">
         <f ca="1">ROUND(RAND()*(2-VALUE(I20))+VALUE(I20),2)</f>
-        <v>1.76</v>
+        <v>1.65</v>
       </c>
       <c r="J21" s="10">
         <f ca="1">ROUND(RAND()*(200-VALUE(J20))+VALUE(J20),2)</f>
-        <v>79.16</v>
+        <v>43.18</v>
       </c>
       <c r="K21" s="9" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="L21" s="10" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="M21" s="10">
         <v>110</v>
@@ -2486,14 +2342,8 @@
       <c r="P21" s="10">
         <v>55</v>
       </c>
-      <c r="Q21" s="10"/>
-      <c r="R21" s="10"/>
-      <c r="S21" s="10"/>
-      <c r="T21" s="10"/>
-      <c r="U21" s="10"/>
-      <c r="V21" s="4"/>
-    </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
         <v>13</v>
       </c>
@@ -2504,30 +2354,30 @@
         <v>13</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="E22" s="9" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="F22" s="9" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="G22" s="9" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="H22" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="I22" s="9">
         <f ca="1">ROUND(RAND()*(0.5-0.3)+0.3, 2)</f>
-        <v>0.34</v>
+        <v>0.39</v>
       </c>
       <c r="J22" s="9">
         <f ca="1">ROUND(RAND()*(10 -1)+1,2)</f>
-        <v>1.48</v>
+        <v>6.28</v>
       </c>
       <c r="K22" s="9" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="L22" s="9" t="s">
         <v>47</v>
@@ -2544,14 +2394,8 @@
       <c r="P22" s="9">
         <v>55</v>
       </c>
-      <c r="Q22" s="9"/>
-      <c r="R22" s="9"/>
-      <c r="S22" s="9"/>
-      <c r="T22" s="9"/>
-      <c r="U22" s="9"/>
-      <c r="V22" s="2"/>
-    </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="10" t="s">
         <v>47</v>
       </c>
@@ -2562,33 +2406,33 @@
         <v>47</v>
       </c>
       <c r="D23" s="10" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="E23" s="10" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="F23" s="10" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="G23" s="10" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="H23" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="I23" s="10">
         <f ca="1">ROUND(RAND()*(1-VALUE(I22))+VALUE(I22),2)</f>
-        <v>0.59</v>
+        <v>0.64</v>
       </c>
       <c r="J23" s="10">
         <f ca="1">ROUND(RAND()*(100-VALUE(J22))+VALUE(J22),2)</f>
-        <v>45.73</v>
+        <v>31.57</v>
       </c>
       <c r="K23" s="9" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="L23" s="10" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="M23" s="10">
         <v>63</v>
@@ -2602,14 +2446,8 @@
       <c r="P23" s="10">
         <v>70</v>
       </c>
-      <c r="Q23" s="10"/>
-      <c r="R23" s="10"/>
-      <c r="S23" s="10"/>
-      <c r="T23" s="10"/>
-      <c r="U23" s="10"/>
-      <c r="V23" s="4"/>
-    </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
         <v>14</v>
       </c>
@@ -2620,30 +2458,30 @@
         <v>14</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="E24" s="9" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="F24" s="9" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="G24" s="9" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="H24" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="I24" s="9">
         <f ca="1">ROUND(RAND()*(0.5-0.3)+0.3, 2)</f>
-        <v>0.5</v>
+        <v>0.43</v>
       </c>
       <c r="J24" s="9">
         <f ca="1">ROUND(RAND()*(10 -1)+1,2)</f>
-        <v>6.8</v>
+        <v>7.47</v>
       </c>
       <c r="K24" s="9" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="L24" s="9" t="s">
         <v>48</v>
@@ -2660,14 +2498,8 @@
       <c r="P24" s="9">
         <v>65</v>
       </c>
-      <c r="Q24" s="9"/>
-      <c r="R24" s="9"/>
-      <c r="S24" s="9"/>
-      <c r="T24" s="9"/>
-      <c r="U24" s="9"/>
-      <c r="V24" s="2"/>
-    </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="10" t="s">
         <v>48</v>
       </c>
@@ -2678,33 +2510,33 @@
         <v>48</v>
       </c>
       <c r="D25" s="10" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="E25" s="10" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="F25" s="10" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="G25" s="10" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="H25" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="I25" s="10">
         <f ca="1">ROUND(RAND()*(1-VALUE(I24))+VALUE(I24),2)</f>
-        <v>0.94</v>
+        <v>0.8</v>
       </c>
       <c r="J25" s="10">
         <f ca="1">ROUND(RAND()*(100-VALUE(J24))+VALUE(J24),2)</f>
-        <v>94.06</v>
+        <v>45.6</v>
       </c>
       <c r="K25" s="9" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="L25" s="10" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="M25" s="10">
         <v>65</v>
@@ -2718,48 +2550,42 @@
       <c r="P25" s="10">
         <v>85</v>
       </c>
-      <c r="Q25" s="10"/>
-      <c r="R25" s="10"/>
-      <c r="S25" s="10"/>
-      <c r="T25" s="10"/>
-      <c r="U25" s="10"/>
-      <c r="V25" s="4"/>
-    </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="B26" s="9">
         <v>25</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="E26" s="9" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="F26" s="9" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="G26" s="9" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="H26" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="I26" s="9">
         <f ca="1">ROUND(RAND()*(0.6-0.3)+0.3, 2)</f>
-        <v>0.44</v>
+        <v>0.39</v>
       </c>
       <c r="J26" s="9">
         <f ca="1">ROUND(RAND()*(10 -1)+1,2)</f>
-        <v>3.96</v>
+        <v>3.39</v>
       </c>
       <c r="K26" s="9" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="L26" s="9" t="s">
         <v>33</v>
@@ -2776,51 +2602,45 @@
       <c r="P26" s="9">
         <v>100</v>
       </c>
-      <c r="Q26" s="9"/>
-      <c r="R26" s="9"/>
-      <c r="S26" s="9"/>
-      <c r="T26" s="9"/>
-      <c r="U26" s="9"/>
-      <c r="V26" s="2"/>
-    </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" s="10" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="B27" s="10">
         <v>26</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="D27" s="10" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="E27" s="10" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="F27" s="10" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="G27" s="10" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="H27" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="I27" s="10">
         <f ca="1">ROUND(RAND()*(1.2-VALUE(I26))+VALUE(I26),2)</f>
-        <v>0.72</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="J27" s="10">
         <f ca="1">ROUND(RAND()*(100-VALUE(J26))+VALUE(J26),2)</f>
-        <v>77.23</v>
+        <v>16.170000000000002</v>
       </c>
       <c r="K27" s="9" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="L27" s="10" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="M27" s="10">
         <v>100</v>
@@ -2834,14 +2654,8 @@
       <c r="P27" s="10">
         <v>120</v>
       </c>
-      <c r="Q27" s="10"/>
-      <c r="R27" s="10"/>
-      <c r="S27" s="10"/>
-      <c r="T27" s="10"/>
-      <c r="U27" s="10"/>
-      <c r="V27" s="4"/>
-    </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
         <v>36</v>
       </c>
@@ -2852,30 +2666,30 @@
         <v>36</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="E28" s="9" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="F28" s="9" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="G28" s="9" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="H28" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="I28" s="9">
         <f ca="1">ROUND(RAND()*(0.6-0.3)+0.3, 2)</f>
-        <v>0.45</v>
+        <v>0.41</v>
       </c>
       <c r="J28" s="9">
         <f ca="1">ROUND(RAND()*(10 -1)+1,2)</f>
-        <v>6.35</v>
+        <v>9.41</v>
       </c>
       <c r="K28" s="9" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="L28" s="9" t="s">
         <v>35</v>
@@ -2892,14 +2706,8 @@
       <c r="P28" s="9">
         <v>50</v>
       </c>
-      <c r="Q28" s="9"/>
-      <c r="R28" s="9"/>
-      <c r="S28" s="9"/>
-      <c r="T28" s="9"/>
-      <c r="U28" s="9"/>
-      <c r="V28" s="2"/>
-    </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" s="10" t="s">
         <v>35</v>
       </c>
@@ -2910,33 +2718,33 @@
         <v>35</v>
       </c>
       <c r="D29" s="10" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="E29" s="10" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="F29" s="10" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="G29" s="10" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="H29" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="I29" s="10">
         <f ca="1">ROUND(RAND()*(0.9-VALUE(I28))+VALUE(I28),2)</f>
-        <v>0.85</v>
+        <v>0.64</v>
       </c>
       <c r="J29" s="10">
         <f ca="1">ROUND(RAND()*(100-VALUE(J28))+VALUE(J28),2)</f>
-        <v>39.409999999999997</v>
+        <v>97.61</v>
       </c>
       <c r="K29" s="10" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="L29" s="10" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="M29" s="10">
         <v>60</v>
@@ -2950,14 +2758,8 @@
       <c r="P29" s="10">
         <v>90</v>
       </c>
-      <c r="Q29" s="10"/>
-      <c r="R29" s="10"/>
-      <c r="S29" s="10"/>
-      <c r="T29" s="10"/>
-      <c r="U29" s="10"/>
-      <c r="V29" s="4"/>
-    </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
         <v>37</v>
       </c>
@@ -2968,30 +2770,30 @@
         <v>37</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="E30" s="9" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="F30" s="9" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="G30" s="9" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="H30" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="I30" s="9">
         <f ca="1">ROUND(RAND()*(0.8-0.3)+0.3, 2)</f>
-        <v>0.43</v>
+        <v>0.67</v>
       </c>
       <c r="J30" s="9">
         <f ca="1">ROUND(RAND()*(10 -1)+1,2)</f>
-        <v>7.76</v>
+        <v>1.21</v>
       </c>
       <c r="K30" s="9" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="L30" s="9" t="s">
         <v>22</v>
@@ -3008,14 +2810,8 @@
       <c r="P30" s="9">
         <v>70</v>
       </c>
-      <c r="Q30" s="9"/>
-      <c r="R30" s="9"/>
-      <c r="S30" s="9"/>
-      <c r="T30" s="9"/>
-      <c r="U30" s="9"/>
-      <c r="V30" s="2"/>
-    </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" s="10" t="s">
         <v>22</v>
       </c>
@@ -3026,33 +2822,33 @@
         <v>22</v>
       </c>
       <c r="D31" s="10" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="E31" s="10" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="F31" s="10" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="G31" s="10" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="H31" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="I31" s="10">
         <f ca="1">ROUND(RAND()*(2-VALUE(I30))+VALUE(I30),2)</f>
-        <v>1.81</v>
+        <v>1.07</v>
       </c>
       <c r="J31" s="10">
         <f ca="1">ROUND(RAND()*(100-VALUE(J30))+VALUE(J30),2)</f>
-        <v>77.63</v>
+        <v>10.28</v>
       </c>
       <c r="K31" s="10" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="L31" s="10" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="M31" s="10">
         <v>60</v>
@@ -3066,14 +2862,8 @@
       <c r="P31" s="10">
         <v>100</v>
       </c>
-      <c r="Q31" s="10"/>
-      <c r="R31" s="10"/>
-      <c r="S31" s="10"/>
-      <c r="T31" s="10"/>
-      <c r="U31" s="10"/>
-      <c r="V31" s="4"/>
-    </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
         <v>4</v>
       </c>
@@ -3084,30 +2874,30 @@
         <v>4</v>
       </c>
       <c r="D32" s="9" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="E32" s="9" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="F32" s="9" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="G32" s="9" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="H32" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="I32" s="9">
         <f ca="1">ROUND(RAND()*(0.5-0.3)+0.3, 2)</f>
-        <v>0.41</v>
+        <v>0.35</v>
       </c>
       <c r="J32" s="9">
         <f ca="1">ROUND(RAND()*(10 -1)+1,2)</f>
-        <v>2.48</v>
+        <v>6.17</v>
       </c>
       <c r="K32" s="9" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="L32" s="9" t="s">
         <v>39</v>
@@ -3124,14 +2914,8 @@
       <c r="P32" s="9">
         <v>45</v>
       </c>
-      <c r="Q32" s="9"/>
-      <c r="R32" s="9"/>
-      <c r="S32" s="9"/>
-      <c r="T32" s="9"/>
-      <c r="U32" s="9"/>
-      <c r="V32" s="2"/>
-    </row>
-    <row r="33" spans="1:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>39</v>
       </c>
@@ -3142,30 +2926,30 @@
         <v>39</v>
       </c>
       <c r="D33" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="E33" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="F33" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="G33" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="H33" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="I33" s="10">
         <f ca="1">ROUND(RAND()*(0.8-VALUE(I32))+VALUE(I32),2)</f>
-        <v>0.44</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="J33" s="10">
         <f ca="1">ROUND(RAND()*(100-VALUE(J32))+VALUE(J32),2)</f>
-        <v>68.22</v>
+        <v>82.49</v>
       </c>
       <c r="K33" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="L33" t="s">
         <v>38</v>
@@ -3182,9 +2966,8 @@
       <c r="P33">
         <v>60</v>
       </c>
-      <c r="V33" s="6"/>
-    </row>
-    <row r="34" spans="1:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" s="10" t="s">
         <v>38</v>
       </c>
@@ -3195,33 +2978,33 @@
         <v>38</v>
       </c>
       <c r="D34" s="10" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="E34" s="10" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="F34" s="10" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="G34" s="10" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="H34" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="I34" s="10">
         <f ca="1">ROUND(RAND()*(2-VALUE(I33))+VALUE(I33),2)</f>
-        <v>1.82</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="J34" s="10">
         <f ca="1">ROUND(RAND()*(200-VALUE(J33))+VALUE(J33),2)</f>
-        <v>199.8</v>
+        <v>171.97</v>
       </c>
       <c r="K34" s="10" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="L34" s="10" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="M34" s="10">
         <v>80</v>
@@ -3235,14 +3018,8 @@
       <c r="P34" s="10">
         <v>120</v>
       </c>
-      <c r="Q34" s="10"/>
-      <c r="R34" s="10"/>
-      <c r="S34" s="10"/>
-      <c r="T34" s="10"/>
-      <c r="U34" s="10"/>
-      <c r="V34" s="4"/>
-    </row>
-    <row r="35" spans="1:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" s="9" t="s">
         <v>40</v>
       </c>
@@ -3253,30 +3030,30 @@
         <v>40</v>
       </c>
       <c r="D35" s="9" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="E35" s="9" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="F35" s="9" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="G35" s="9" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="H35" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="I35" s="9">
         <f ca="1">ROUND(RAND()*(1-0.3)+0.3, 2)</f>
-        <v>0.4</v>
+        <v>0.67</v>
       </c>
       <c r="J35" s="9">
         <f ca="1">ROUND(RAND()*(10 -1)+1,2)</f>
-        <v>3.72</v>
+        <v>9.3800000000000008</v>
       </c>
       <c r="K35" s="9" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="L35" s="9" t="s">
         <v>41</v>
@@ -3293,14 +3070,8 @@
       <c r="P35" s="9">
         <v>80</v>
       </c>
-      <c r="Q35" s="9"/>
-      <c r="R35" s="9"/>
-      <c r="S35" s="9"/>
-      <c r="T35" s="9"/>
-      <c r="U35" s="9"/>
-      <c r="V35" s="2"/>
-    </row>
-    <row r="36" spans="1:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" s="10" t="s">
         <v>41</v>
       </c>
@@ -3311,33 +3082,33 @@
         <v>41</v>
       </c>
       <c r="D36" s="10" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="E36" s="10" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="F36" s="10" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="G36" s="10" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="H36" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="I36" s="10">
         <f ca="1">ROUND(RAND()*(1-VALUE(I35))+VALUE(I35),2)</f>
-        <v>0.77</v>
+        <v>0.7</v>
       </c>
       <c r="J36" s="10">
         <f ca="1">ROUND(RAND()*(100-VALUE(J35))+VALUE(J35),2)</f>
-        <v>4.8899999999999997</v>
+        <v>89.2</v>
       </c>
       <c r="K36" s="10" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="L36" s="10" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="M36" s="10">
         <v>50</v>
@@ -3351,14 +3122,8 @@
       <c r="P36" s="10">
         <v>90</v>
       </c>
-      <c r="Q36" s="10"/>
-      <c r="R36" s="10"/>
-      <c r="S36" s="10"/>
-      <c r="T36" s="10"/>
-      <c r="U36" s="10"/>
-      <c r="V36" s="4"/>
-    </row>
-    <row r="37" spans="1:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" s="9" t="s">
         <v>43</v>
       </c>
@@ -3369,30 +3134,30 @@
         <v>43</v>
       </c>
       <c r="D37" s="9" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="E37" s="9" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="F37" s="9" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="G37" s="9" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="H37" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="I37" s="9">
         <f ca="1">ROUND(RAND()*(0.8-0.3)+0.3, 2)</f>
-        <v>0.44</v>
+        <v>0.43</v>
       </c>
       <c r="J37" s="9">
         <f ca="1">ROUND(RAND()*(10 -1)+1,2)</f>
-        <v>1.84</v>
+        <v>1.06</v>
       </c>
       <c r="K37" s="9" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="L37" s="9" t="s">
         <v>42</v>
@@ -3409,14 +3174,8 @@
       <c r="P37" s="9">
         <v>30</v>
       </c>
-      <c r="Q37" s="9"/>
-      <c r="R37" s="9"/>
-      <c r="S37" s="9"/>
-      <c r="T37" s="9"/>
-      <c r="U37" s="9"/>
-      <c r="V37" s="2"/>
-    </row>
-    <row r="38" spans="1:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" s="10" t="s">
         <v>42</v>
       </c>
@@ -3427,33 +3186,33 @@
         <v>42</v>
       </c>
       <c r="D38" s="10" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="E38" s="10" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="F38" s="10" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="G38" s="10" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="H38" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="I38" s="10">
         <f ca="1">ROUND(RAND()*(1.4-VALUE(I37))+VALUE(I37),2)</f>
-        <v>0.46</v>
+        <v>1.05</v>
       </c>
       <c r="J38" s="10">
         <f ca="1">ROUND(RAND()*(100-VALUE(J37))+VALUE(J37),2)</f>
-        <v>49.19</v>
+        <v>32.020000000000003</v>
       </c>
       <c r="K38" s="10" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="L38" s="10" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="M38" s="10">
         <v>70</v>
@@ -3467,14 +3226,8 @@
       <c r="P38" s="10">
         <v>40</v>
       </c>
-      <c r="Q38" s="10"/>
-      <c r="R38" s="10"/>
-      <c r="S38" s="10"/>
-      <c r="T38" s="10"/>
-      <c r="U38" s="10"/>
-      <c r="V38" s="4"/>
-    </row>
-    <row r="39" spans="1:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" s="9" t="s">
         <v>44</v>
       </c>
@@ -3485,29 +3238,29 @@
         <v>44</v>
       </c>
       <c r="D39" s="9" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="E39" s="9" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="F39" s="9" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="G39" s="9" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="H39" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="I39" s="9">
         <v>0.6</v>
       </c>
       <c r="J39" s="9">
         <f ca="1">ROUND(RAND()*(10 -1)+1,2)</f>
-        <v>6.17</v>
+        <v>6.41</v>
       </c>
       <c r="K39" s="9" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="L39" s="9" t="s">
         <v>45</v>
@@ -3524,14 +3277,8 @@
       <c r="P39" s="9">
         <v>60</v>
       </c>
-      <c r="Q39" s="9"/>
-      <c r="R39" s="9"/>
-      <c r="S39" s="9"/>
-      <c r="T39" s="9"/>
-      <c r="U39" s="9"/>
-      <c r="V39" s="2"/>
-    </row>
-    <row r="40" spans="1:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" s="10" t="s">
         <v>45</v>
       </c>
@@ -3542,33 +3289,33 @@
         <v>45</v>
       </c>
       <c r="D40" s="10" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="E40" s="10" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="F40" s="10" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="G40" s="10" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="H40" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="I40" s="10">
         <f ca="1">ROUND(RAND()*(1.2-VALUE(I39))+VALUE(I39),2)</f>
-        <v>0.97</v>
+        <v>0.82</v>
       </c>
       <c r="J40" s="10">
         <f ca="1">ROUND(RAND()*(100-VALUE(J39))+VALUE(J39),2)</f>
-        <v>30.35</v>
+        <v>56.31</v>
       </c>
       <c r="K40" s="10" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="L40" s="10" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="M40" s="10">
         <v>70</v>
@@ -3582,14 +3329,8 @@
       <c r="P40" s="10">
         <v>90</v>
       </c>
-      <c r="Q40" s="10"/>
-      <c r="R40" s="10"/>
-      <c r="S40" s="10"/>
-      <c r="T40" s="10"/>
-      <c r="U40" s="10"/>
-      <c r="V40" s="4"/>
-    </row>
-    <row r="41" spans="1:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" s="11" t="s">
         <v>3</v>
       </c>
@@ -3600,33 +3341,33 @@
         <v>3</v>
       </c>
       <c r="D41" s="11" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="E41" s="11" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="F41" s="11" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="G41" s="11" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="H41" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="I41" s="11">
         <f ca="1">ROUND(RAND()*(0.5-0.3)+0.3, 2)</f>
-        <v>0.35</v>
+        <v>0.41</v>
       </c>
       <c r="J41" s="9">
         <f ca="1">ROUND(RAND()*(10 -1)+1,2)</f>
-        <v>2.34</v>
+        <v>6.6</v>
       </c>
       <c r="K41" s="11" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="L41" s="11" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="M41" s="11">
         <v>40</v>
@@ -3640,14 +3381,8 @@
       <c r="P41" s="11">
         <v>30</v>
       </c>
-      <c r="Q41" s="11"/>
-      <c r="R41" s="11"/>
-      <c r="S41" s="11"/>
-      <c r="T41" s="11"/>
-      <c r="U41" s="11"/>
-      <c r="V41" s="8"/>
-    </row>
-    <row r="42" spans="1:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" s="11" t="s">
         <v>5</v>
       </c>
@@ -3658,33 +3393,33 @@
         <v>5</v>
       </c>
       <c r="D42" s="11" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="E42" s="11" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="F42" s="11" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="G42" s="11" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="H42" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="I42" s="11">
         <f ca="1">ROUND(RAND()*(0.5-0.3)+0.3, 2)</f>
-        <v>0.36</v>
+        <v>0.4</v>
       </c>
       <c r="J42" s="9">
         <f ca="1">ROUND(RAND()*(10 -1)+1,2)</f>
-        <v>9.77</v>
+        <v>2.33</v>
       </c>
       <c r="K42" s="11" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="L42" s="11" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="M42" s="11">
         <v>40</v>
@@ -3698,14 +3433,8 @@
       <c r="P42" s="11">
         <v>40</v>
       </c>
-      <c r="Q42" s="11"/>
-      <c r="R42" s="11"/>
-      <c r="S42" s="11"/>
-      <c r="T42" s="11"/>
-      <c r="U42" s="11"/>
-      <c r="V42" s="8"/>
-    </row>
-    <row r="43" spans="1:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" s="9" t="s">
         <v>20</v>
       </c>
@@ -3716,30 +3445,30 @@
         <v>20</v>
       </c>
       <c r="D43" s="9" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="E43" s="9" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="F43" s="9" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="G43" s="9" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="H43" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="I43" s="9">
         <f ca="1">ROUND(RAND()*(2-1)+1, 2)</f>
-        <v>1.24</v>
+        <v>1.89</v>
       </c>
       <c r="J43" s="9">
         <f ca="1">ROUND(RAND()*(10 -1)+1,2)</f>
-        <v>5.87</v>
+        <v>7.4</v>
       </c>
       <c r="K43" s="9" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="L43" s="9" t="s">
         <v>19</v>
@@ -3756,14 +3485,8 @@
       <c r="P43" s="9">
         <v>60</v>
       </c>
-      <c r="Q43" s="9"/>
-      <c r="R43" s="9"/>
-      <c r="S43" s="9"/>
-      <c r="T43" s="9"/>
-      <c r="U43" s="9"/>
-      <c r="V43" s="2"/>
-    </row>
-    <row r="44" spans="1:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44" s="10" t="s">
         <v>19</v>
       </c>
@@ -3774,33 +3497,33 @@
         <v>19</v>
       </c>
       <c r="D44" s="10" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="E44" s="10" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="F44" s="10" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="G44" s="10" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="H44" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="I44" s="10">
         <f ca="1">ROUND(RAND()*(2-VALUE(I43))+VALUE(I43),2)</f>
-        <v>1.46</v>
+        <v>1.9</v>
       </c>
       <c r="J44" s="10">
         <f ca="1">ROUND(RAND()*(100-VALUE(J43))+VALUE(J43),2)</f>
-        <v>47.02</v>
+        <v>57.07</v>
       </c>
       <c r="K44" s="10" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="L44" s="10" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="M44" s="10">
         <v>80</v>
@@ -3814,14 +3537,8 @@
       <c r="P44" s="10">
         <v>90</v>
       </c>
-      <c r="Q44" s="10"/>
-      <c r="R44" s="10"/>
-      <c r="S44" s="10"/>
-      <c r="T44" s="10"/>
-      <c r="U44" s="10"/>
-      <c r="V44" s="4"/>
-    </row>
-    <row r="45" spans="1:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" s="11" t="s">
         <v>23</v>
       </c>
@@ -3832,33 +3549,33 @@
         <v>23</v>
       </c>
       <c r="D45" s="11" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="E45" s="11" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="F45" s="11" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="G45" s="11" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="H45" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="I45" s="9">
         <f ca="1">ROUND(RAND()*(2-1)+1, 2)</f>
-        <v>1.53</v>
+        <v>1.03</v>
       </c>
       <c r="J45" s="9">
         <f t="shared" ref="J45:J50" ca="1" si="0">ROUND(RAND()*(10 -1)+1,2)</f>
-        <v>5.43</v>
+        <v>8.11</v>
       </c>
       <c r="K45" s="11" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="L45" s="11" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="M45" s="11">
         <v>100</v>
@@ -3872,14 +3589,8 @@
       <c r="P45" s="11">
         <v>100</v>
       </c>
-      <c r="Q45" s="11"/>
-      <c r="R45" s="11"/>
-      <c r="S45" s="11"/>
-      <c r="T45" s="11"/>
-      <c r="U45" s="11"/>
-      <c r="V45" s="8"/>
-    </row>
-    <row r="46" spans="1:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46" s="11" t="s">
         <v>25</v>
       </c>
@@ -3890,33 +3601,33 @@
         <v>25</v>
       </c>
       <c r="D46" s="11" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="E46" s="11" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="F46" s="11" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="G46" s="11" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="H46" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="I46" s="9">
         <f ca="1">ROUND(RAND()*(2-1)+1, 2)</f>
-        <v>1.04</v>
+        <v>1.9</v>
       </c>
       <c r="J46" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>3.98</v>
+        <v>1.26</v>
       </c>
       <c r="K46" s="11" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="L46" s="11" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="M46" s="11">
         <v>80</v>
@@ -3930,14 +3641,8 @@
       <c r="P46" s="11">
         <v>110</v>
       </c>
-      <c r="Q46" s="11"/>
-      <c r="R46" s="11"/>
-      <c r="S46" s="11"/>
-      <c r="T46" s="11"/>
-      <c r="U46" s="11"/>
-      <c r="V46" s="8"/>
-    </row>
-    <row r="47" spans="1:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A47" s="11" t="s">
         <v>26</v>
       </c>
@@ -3948,33 +3653,33 @@
         <v>26</v>
       </c>
       <c r="D47" s="11" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="E47" s="11" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="F47" s="11" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="G47" s="11" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="H47" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="I47" s="9">
         <f ca="1">ROUND(RAND()*(2-1)+1, 2)</f>
-        <v>1.17</v>
+        <v>1.76</v>
       </c>
       <c r="J47" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>4.1900000000000004</v>
+        <v>7.63</v>
       </c>
       <c r="K47" s="11" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="L47" s="11" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="M47" s="11">
         <v>60</v>
@@ -3988,14 +3693,8 @@
       <c r="P47" s="11">
         <v>60</v>
       </c>
-      <c r="Q47" s="11"/>
-      <c r="R47" s="11"/>
-      <c r="S47" s="11"/>
-      <c r="T47" s="11"/>
-      <c r="U47" s="11"/>
-      <c r="V47" s="8"/>
-    </row>
-    <row r="48" spans="1:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A48" s="11" t="s">
         <v>31</v>
       </c>
@@ -4006,33 +3705,33 @@
         <v>31</v>
       </c>
       <c r="D48" s="11" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="E48" s="11" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="F48" s="11" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="G48" s="11" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="H48" s="11" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="I48" s="9">
         <f ca="1">ROUND(RAND()*(2-1)+1, 2)</f>
-        <v>1.98</v>
+        <v>1.88</v>
       </c>
       <c r="J48" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>2.5299999999999998</v>
+        <v>7.52</v>
       </c>
       <c r="K48" s="11" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="L48" s="11" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="M48" s="11">
         <v>60</v>
@@ -4046,14 +3745,8 @@
       <c r="P48" s="11">
         <v>110</v>
       </c>
-      <c r="Q48" s="11"/>
-      <c r="R48" s="11"/>
-      <c r="S48" s="11"/>
-      <c r="T48" s="11"/>
-      <c r="U48" s="11"/>
-      <c r="V48" s="8"/>
-    </row>
-    <row r="49" spans="1:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A49" s="11" t="s">
         <v>46</v>
       </c>
@@ -4064,33 +3757,33 @@
         <v>46</v>
       </c>
       <c r="D49" s="11" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="E49" s="11" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="F49" s="11" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="G49" s="11" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="H49" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="I49" s="11">
         <f ca="1">ROUND(RAND()*(1.4-1)+1, 2)</f>
-        <v>1.23</v>
+        <v>1.03</v>
       </c>
       <c r="J49" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>5.53</v>
+        <v>7.12</v>
       </c>
       <c r="K49" s="11" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="L49" s="11" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="M49" s="11">
         <v>80</v>
@@ -4104,14 +3797,8 @@
       <c r="P49" s="11">
         <v>120</v>
       </c>
-      <c r="Q49" s="11"/>
-      <c r="R49" s="11"/>
-      <c r="S49" s="11"/>
-      <c r="T49" s="11"/>
-      <c r="U49" s="11"/>
-      <c r="V49" s="8"/>
-    </row>
-    <row r="50" spans="1:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50" s="10" t="s">
         <v>15</v>
       </c>
@@ -4122,33 +3809,33 @@
         <v>15</v>
       </c>
       <c r="D50" s="10" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="E50" s="10" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="F50" s="10" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="G50" s="10" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="H50" s="10" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="I50" s="10">
         <f ca="1">ROUND(RAND()*(0.5-0.3)+0.3, 2)</f>
-        <v>0.45</v>
+        <v>0.35</v>
       </c>
       <c r="J50" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>6.3</v>
+        <v>4.9400000000000004</v>
       </c>
       <c r="K50" s="10" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="L50" s="10" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="M50" s="10">
         <v>40</v>
@@ -4162,12 +3849,6 @@
       <c r="P50" s="10">
         <v>40</v>
       </c>
-      <c r="Q50" s="10"/>
-      <c r="R50" s="10"/>
-      <c r="S50" s="10"/>
-      <c r="T50" s="10"/>
-      <c r="U50" s="10"/>
-      <c r="V50" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
non important changes to data
</commit_message>
<xml_diff>
--- a/Content/_Data/Pokemon/pokemon-data.xlsx
+++ b/Content/_Data/Pokemon/pokemon-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Unreal\PokemonRemake\Content\_Data\Pokemon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{299745D1-0DC3-434E-A81F-4400816E0ABD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8538D2F-4BE8-4405-9EE4-197FA91605CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57495" yWindow="0" windowWidth="19410" windowHeight="20985" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main-Data" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="555" uniqueCount="253">
   <si>
     <t>Alien</t>
   </si>
@@ -1243,8 +1243,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55723188-F4D3-4EF4-AEA8-7A04D3578F8F}">
   <dimension ref="A1:P50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="Q1" sqref="Q1:V1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1335,11 +1335,11 @@
       </c>
       <c r="I2" s="9">
         <f ca="1">ROUND(RAND()*(0.6-0.3)+0.3, 2)</f>
-        <v>0.43</v>
+        <v>0.39</v>
       </c>
       <c r="J2" s="9">
         <f ca="1">ROUND(RAND()*(10 -1)+1,2)</f>
-        <v>1.92</v>
+        <v>5.89</v>
       </c>
       <c r="K2" s="9" t="s">
         <v>177</v>
@@ -1387,11 +1387,11 @@
       </c>
       <c r="I3" s="10">
         <f ca="1">ROUND(RAND()*(2-VALUE(I2))+VALUE(I2),2)</f>
-        <v>1</v>
+        <v>1.19</v>
       </c>
       <c r="J3" s="10">
         <f ca="1">ROUND(RAND()*(100-VALUE(J2))+VALUE(J2),2)</f>
-        <v>33.42</v>
+        <v>39.03</v>
       </c>
       <c r="K3" s="9" t="s">
         <v>177</v>
@@ -1439,11 +1439,11 @@
       </c>
       <c r="I4" s="9">
         <f ca="1">ROUND(RAND()*(0.6-0.3)+0.3, 2)</f>
-        <v>0.54</v>
+        <v>0.32</v>
       </c>
       <c r="J4" s="9">
         <f ca="1">ROUND(RAND()*(10 -1)+1,2)</f>
-        <v>9.68</v>
+        <v>3</v>
       </c>
       <c r="K4" s="9" t="s">
         <v>179</v>
@@ -1491,11 +1491,11 @@
       </c>
       <c r="I5" s="10">
         <f ca="1">ROUND(RAND()*(2-VALUE(I4))+VALUE(I4),2)</f>
-        <v>1.47</v>
+        <v>1.4</v>
       </c>
       <c r="J5" s="10">
         <f ca="1">ROUND(RAND()*(100-VALUE(J4))+VALUE(J4),2)</f>
-        <v>21.6</v>
+        <v>90.25</v>
       </c>
       <c r="K5" s="9" t="s">
         <v>179</v>
@@ -1543,11 +1543,11 @@
       </c>
       <c r="I6" s="9">
         <f ca="1">ROUND(RAND()*(0.8-0.3)+0.3, 2)</f>
-        <v>0.69</v>
+        <v>0.33</v>
       </c>
       <c r="J6" s="9">
         <f ca="1">ROUND(RAND()*(10 -1)+1,2)</f>
-        <v>3.9</v>
+        <v>4.8099999999999996</v>
       </c>
       <c r="K6" s="9" t="s">
         <v>180</v>
@@ -1595,11 +1595,11 @@
       </c>
       <c r="I7" s="10">
         <f ca="1">ROUND(RAND()*(2-VALUE(I6))+VALUE(I6),2)</f>
-        <v>1.46</v>
+        <v>1.87</v>
       </c>
       <c r="J7" s="10">
         <f ca="1">ROUND(RAND()*(100-VALUE(J6))+VALUE(J6),2)</f>
-        <v>88.97</v>
+        <v>70.97</v>
       </c>
       <c r="K7" s="9" t="s">
         <v>180</v>
@@ -1647,11 +1647,11 @@
       </c>
       <c r="I8" s="9">
         <f ca="1">ROUND(RAND()*(0.5-0.3)+0.3, 2)</f>
-        <v>0.49</v>
+        <v>0.43</v>
       </c>
       <c r="J8" s="9">
         <f ca="1">ROUND(RAND()*(10 -1)+1,2)</f>
-        <v>7.02</v>
+        <v>2.93</v>
       </c>
       <c r="K8" s="9" t="s">
         <v>182</v>
@@ -1699,11 +1699,11 @@
       </c>
       <c r="I9" s="10">
         <f ca="1">ROUND(RAND()*(2-VALUE(I8))+VALUE(I8),2)</f>
-        <v>1.49</v>
+        <v>1.69</v>
       </c>
       <c r="J9" s="10">
         <f ca="1">ROUND(RAND()*(100-VALUE(J8))+VALUE(J8),2)</f>
-        <v>91.23</v>
+        <v>64.84</v>
       </c>
       <c r="K9" s="9" t="s">
         <v>182</v>
@@ -1751,7 +1751,7 @@
       </c>
       <c r="I10" s="9">
         <f ca="1">ROUND(RAND()*(0.5-0.3)+0.3, 2)</f>
-        <v>0.44</v>
+        <v>0.33</v>
       </c>
       <c r="J10" s="9">
         <v>10.3</v>
@@ -1802,7 +1802,7 @@
       </c>
       <c r="I11" s="10">
         <f ca="1">ROUND(RAND()*(2-VALUE(I10))+VALUE(I10),2)</f>
-        <v>1.52</v>
+        <v>1.21</v>
       </c>
       <c r="J11" s="10">
         <v>25.4</v>
@@ -1853,7 +1853,7 @@
       </c>
       <c r="I12" s="9">
         <f ca="1">ROUND(RAND()*(0.64-0.3)+0.3, 2)</f>
-        <v>0.49</v>
+        <v>0.47</v>
       </c>
       <c r="J12" s="9">
         <v>1</v>
@@ -1904,7 +1904,7 @@
       </c>
       <c r="I13">
         <f ca="1">ROUND(RAND()*(1-VALUE(I12))+VALUE(I12),2)</f>
-        <v>0.85</v>
+        <v>0.82</v>
       </c>
       <c r="J13">
         <v>4.5</v>
@@ -1955,7 +1955,7 @@
       </c>
       <c r="I14" s="10">
         <f ca="1">ROUND(RAND()*(2-VALUE(I13))+VALUE(I13),2)</f>
-        <v>1.1000000000000001</v>
+        <v>1.27</v>
       </c>
       <c r="J14" s="10">
         <v>39.200000000000003</v>
@@ -2006,11 +2006,11 @@
       </c>
       <c r="I15">
         <f ca="1">ROUND(RAND()*(0.6-0.3)+0.3, 2)</f>
-        <v>0.5</v>
+        <v>0.51</v>
       </c>
       <c r="J15" s="9">
         <f ca="1">ROUND(RAND()*(10 -1)+1,2)</f>
-        <v>6.84</v>
+        <v>3.85</v>
       </c>
       <c r="K15" s="9" t="s">
         <v>184</v>
@@ -2058,11 +2058,11 @@
       </c>
       <c r="I16" s="10">
         <f ca="1">ROUND(RAND()*(2-1)+1,2)</f>
-        <v>1.1000000000000001</v>
+        <v>1.81</v>
       </c>
       <c r="J16" s="10">
         <f ca="1">ROUND(RAND()*(100-VALUE(J15))+VALUE(J15),2)</f>
-        <v>79.37</v>
+        <v>42.87</v>
       </c>
       <c r="K16" s="9" t="s">
         <v>185</v>
@@ -2110,11 +2110,11 @@
       </c>
       <c r="I17" s="9">
         <f ca="1">ROUND(RAND()*(0.6-0.3)+0.3, 2)</f>
-        <v>0.32</v>
+        <v>0.49</v>
       </c>
       <c r="J17" s="9">
         <f ca="1">ROUND(RAND()*(10 -1)+1,2)</f>
-        <v>5.97</v>
+        <v>9.48</v>
       </c>
       <c r="K17" s="9" t="s">
         <v>187</v>
@@ -2162,11 +2162,11 @@
       </c>
       <c r="I18" s="10">
         <f ca="1">ROUND(RAND()*(2-1)+1,2)</f>
-        <v>1.21</v>
+        <v>1.94</v>
       </c>
       <c r="J18" s="10">
         <f ca="1">ROUND(RAND()*(100-VALUE(J17))+VALUE(J17),2)</f>
-        <v>12.59</v>
+        <v>64.7</v>
       </c>
       <c r="K18" s="9" t="s">
         <v>188</v>
@@ -2214,11 +2214,11 @@
       </c>
       <c r="I19" s="9">
         <f ca="1">ROUND(RAND()*(1-0.3)+0.3, 2)</f>
-        <v>0.56999999999999995</v>
+        <v>0.86</v>
       </c>
       <c r="J19" s="9">
         <f ca="1">ROUND(RAND()*(10 -1)+1,2)</f>
-        <v>1.77</v>
+        <v>1.94</v>
       </c>
       <c r="K19" s="9" t="s">
         <v>252</v>
@@ -2266,11 +2266,11 @@
       </c>
       <c r="I20" s="10">
         <f ca="1">ROUND(RAND()*(2-0.8)+0.8,2)</f>
-        <v>1.37</v>
+        <v>1.8</v>
       </c>
       <c r="J20" s="10">
         <f ca="1">ROUND(RAND()*(100-VALUE(J19))+VALUE(J19),2)</f>
-        <v>15.19</v>
+        <v>63.45</v>
       </c>
       <c r="K20" s="9" t="s">
         <v>251</v>
@@ -2318,11 +2318,11 @@
       </c>
       <c r="I21" s="10">
         <f ca="1">ROUND(RAND()*(2-VALUE(I20))+VALUE(I20),2)</f>
-        <v>1.65</v>
+        <v>2</v>
       </c>
       <c r="J21" s="10">
         <f ca="1">ROUND(RAND()*(200-VALUE(J20))+VALUE(J20),2)</f>
-        <v>43.18</v>
+        <v>176.62</v>
       </c>
       <c r="K21" s="9" t="s">
         <v>251</v>
@@ -2370,11 +2370,11 @@
       </c>
       <c r="I22" s="9">
         <f ca="1">ROUND(RAND()*(0.5-0.3)+0.3, 2)</f>
-        <v>0.39</v>
+        <v>0.49</v>
       </c>
       <c r="J22" s="9">
         <f ca="1">ROUND(RAND()*(10 -1)+1,2)</f>
-        <v>6.28</v>
+        <v>7.94</v>
       </c>
       <c r="K22" s="9" t="s">
         <v>172</v>
@@ -2422,11 +2422,11 @@
       </c>
       <c r="I23" s="10">
         <f ca="1">ROUND(RAND()*(1-VALUE(I22))+VALUE(I22),2)</f>
-        <v>0.64</v>
+        <v>0.76</v>
       </c>
       <c r="J23" s="10">
         <f ca="1">ROUND(RAND()*(100-VALUE(J22))+VALUE(J22),2)</f>
-        <v>31.57</v>
+        <v>55.29</v>
       </c>
       <c r="K23" s="9" t="s">
         <v>172</v>
@@ -2474,11 +2474,11 @@
       </c>
       <c r="I24" s="9">
         <f ca="1">ROUND(RAND()*(0.5-0.3)+0.3, 2)</f>
-        <v>0.43</v>
+        <v>0.47</v>
       </c>
       <c r="J24" s="9">
         <f ca="1">ROUND(RAND()*(10 -1)+1,2)</f>
-        <v>7.47</v>
+        <v>1.97</v>
       </c>
       <c r="K24" s="9" t="s">
         <v>192</v>
@@ -2526,11 +2526,11 @@
       </c>
       <c r="I25" s="10">
         <f ca="1">ROUND(RAND()*(1-VALUE(I24))+VALUE(I24),2)</f>
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="J25" s="10">
         <f ca="1">ROUND(RAND()*(100-VALUE(J24))+VALUE(J24),2)</f>
-        <v>45.6</v>
+        <v>50.23</v>
       </c>
       <c r="K25" s="9" t="s">
         <v>193</v>
@@ -2578,11 +2578,11 @@
       </c>
       <c r="I26" s="9">
         <f ca="1">ROUND(RAND()*(0.6-0.3)+0.3, 2)</f>
-        <v>0.39</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="J26" s="9">
         <f ca="1">ROUND(RAND()*(10 -1)+1,2)</f>
-        <v>3.39</v>
+        <v>8.86</v>
       </c>
       <c r="K26" s="9" t="s">
         <v>194</v>
@@ -2630,11 +2630,11 @@
       </c>
       <c r="I27" s="10">
         <f ca="1">ROUND(RAND()*(1.2-VALUE(I26))+VALUE(I26),2)</f>
-        <v>0.56999999999999995</v>
+        <v>0.77</v>
       </c>
       <c r="J27" s="10">
         <f ca="1">ROUND(RAND()*(100-VALUE(J26))+VALUE(J26),2)</f>
-        <v>16.170000000000002</v>
+        <v>12.55</v>
       </c>
       <c r="K27" s="9" t="s">
         <v>195</v>
@@ -2682,11 +2682,11 @@
       </c>
       <c r="I28" s="9">
         <f ca="1">ROUND(RAND()*(0.6-0.3)+0.3, 2)</f>
-        <v>0.41</v>
+        <v>0.44</v>
       </c>
       <c r="J28" s="9">
         <f ca="1">ROUND(RAND()*(10 -1)+1,2)</f>
-        <v>9.41</v>
+        <v>3.88</v>
       </c>
       <c r="K28" s="9" t="s">
         <v>196</v>
@@ -2734,11 +2734,11 @@
       </c>
       <c r="I29" s="10">
         <f ca="1">ROUND(RAND()*(0.9-VALUE(I28))+VALUE(I28),2)</f>
-        <v>0.64</v>
+        <v>0.83</v>
       </c>
       <c r="J29" s="10">
         <f ca="1">ROUND(RAND()*(100-VALUE(J28))+VALUE(J28),2)</f>
-        <v>97.61</v>
+        <v>19.75</v>
       </c>
       <c r="K29" s="10" t="s">
         <v>198</v>
@@ -2786,11 +2786,11 @@
       </c>
       <c r="I30" s="9">
         <f ca="1">ROUND(RAND()*(0.8-0.3)+0.3, 2)</f>
-        <v>0.67</v>
+        <v>0.45</v>
       </c>
       <c r="J30" s="9">
         <f ca="1">ROUND(RAND()*(10 -1)+1,2)</f>
-        <v>1.21</v>
+        <v>1.17</v>
       </c>
       <c r="K30" s="9" t="s">
         <v>199</v>
@@ -2838,11 +2838,11 @@
       </c>
       <c r="I31" s="10">
         <f ca="1">ROUND(RAND()*(2-VALUE(I30))+VALUE(I30),2)</f>
-        <v>1.07</v>
+        <v>1.42</v>
       </c>
       <c r="J31" s="10">
         <f ca="1">ROUND(RAND()*(100-VALUE(J30))+VALUE(J30),2)</f>
-        <v>10.28</v>
+        <v>89.26</v>
       </c>
       <c r="K31" s="10" t="s">
         <v>199</v>
@@ -2890,11 +2890,11 @@
       </c>
       <c r="I32" s="9">
         <f ca="1">ROUND(RAND()*(0.5-0.3)+0.3, 2)</f>
-        <v>0.35</v>
+        <v>0.46</v>
       </c>
       <c r="J32" s="9">
         <f ca="1">ROUND(RAND()*(10 -1)+1,2)</f>
-        <v>6.17</v>
+        <v>8.26</v>
       </c>
       <c r="K32" s="9" t="s">
         <v>201</v>
@@ -2942,11 +2942,11 @@
       </c>
       <c r="I33" s="10">
         <f ca="1">ROUND(RAND()*(0.8-VALUE(I32))+VALUE(I32),2)</f>
-        <v>0.57999999999999996</v>
+        <v>0.66</v>
       </c>
       <c r="J33" s="10">
         <f ca="1">ROUND(RAND()*(100-VALUE(J32))+VALUE(J32),2)</f>
-        <v>82.49</v>
+        <v>57.46</v>
       </c>
       <c r="K33" t="s">
         <v>204</v>
@@ -2994,11 +2994,11 @@
       </c>
       <c r="I34" s="10">
         <f ca="1">ROUND(RAND()*(2-VALUE(I33))+VALUE(I33),2)</f>
-        <v>1.1200000000000001</v>
+        <v>1.86</v>
       </c>
       <c r="J34" s="10">
         <f ca="1">ROUND(RAND()*(200-VALUE(J33))+VALUE(J33),2)</f>
-        <v>171.97</v>
+        <v>149.41999999999999</v>
       </c>
       <c r="K34" s="10" t="s">
         <v>204</v>
@@ -3046,11 +3046,11 @@
       </c>
       <c r="I35" s="9">
         <f ca="1">ROUND(RAND()*(1-0.3)+0.3, 2)</f>
-        <v>0.67</v>
+        <v>0.35</v>
       </c>
       <c r="J35" s="9">
         <f ca="1">ROUND(RAND()*(10 -1)+1,2)</f>
-        <v>9.3800000000000008</v>
+        <v>1.17</v>
       </c>
       <c r="K35" s="9" t="s">
         <v>175</v>
@@ -3098,11 +3098,11 @@
       </c>
       <c r="I36" s="10">
         <f ca="1">ROUND(RAND()*(1-VALUE(I35))+VALUE(I35),2)</f>
-        <v>0.7</v>
+        <v>0.51</v>
       </c>
       <c r="J36" s="10">
         <f ca="1">ROUND(RAND()*(100-VALUE(J35))+VALUE(J35),2)</f>
-        <v>89.2</v>
+        <v>84.59</v>
       </c>
       <c r="K36" s="10" t="s">
         <v>175</v>
@@ -3150,11 +3150,11 @@
       </c>
       <c r="I37" s="9">
         <f ca="1">ROUND(RAND()*(0.8-0.3)+0.3, 2)</f>
-        <v>0.43</v>
+        <v>0.73</v>
       </c>
       <c r="J37" s="9">
         <f ca="1">ROUND(RAND()*(10 -1)+1,2)</f>
-        <v>1.06</v>
+        <v>6.74</v>
       </c>
       <c r="K37" s="9" t="s">
         <v>207</v>
@@ -3202,11 +3202,11 @@
       </c>
       <c r="I38" s="10">
         <f ca="1">ROUND(RAND()*(1.4-VALUE(I37))+VALUE(I37),2)</f>
-        <v>1.05</v>
+        <v>1.25</v>
       </c>
       <c r="J38" s="10">
         <f ca="1">ROUND(RAND()*(100-VALUE(J37))+VALUE(J37),2)</f>
-        <v>32.020000000000003</v>
+        <v>11.74</v>
       </c>
       <c r="K38" s="10" t="s">
         <v>208</v>
@@ -3257,7 +3257,7 @@
       </c>
       <c r="J39" s="9">
         <f ca="1">ROUND(RAND()*(10 -1)+1,2)</f>
-        <v>6.41</v>
+        <v>8.9600000000000009</v>
       </c>
       <c r="K39" s="9" t="s">
         <v>210</v>
@@ -3305,11 +3305,11 @@
       </c>
       <c r="I40" s="10">
         <f ca="1">ROUND(RAND()*(1.2-VALUE(I39))+VALUE(I39),2)</f>
-        <v>0.82</v>
+        <v>1.2</v>
       </c>
       <c r="J40" s="10">
         <f ca="1">ROUND(RAND()*(100-VALUE(J39))+VALUE(J39),2)</f>
-        <v>56.31</v>
+        <v>87.85</v>
       </c>
       <c r="K40" s="10" t="s">
         <v>211</v>
@@ -3357,11 +3357,11 @@
       </c>
       <c r="I41" s="11">
         <f ca="1">ROUND(RAND()*(0.5-0.3)+0.3, 2)</f>
-        <v>0.41</v>
+        <v>0.47</v>
       </c>
       <c r="J41" s="9">
         <f ca="1">ROUND(RAND()*(10 -1)+1,2)</f>
-        <v>6.6</v>
+        <v>4.3</v>
       </c>
       <c r="K41" s="11" t="s">
         <v>192</v>
@@ -3409,11 +3409,11 @@
       </c>
       <c r="I42" s="11">
         <f ca="1">ROUND(RAND()*(0.5-0.3)+0.3, 2)</f>
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="J42" s="9">
         <f ca="1">ROUND(RAND()*(10 -1)+1,2)</f>
-        <v>2.33</v>
+        <v>5.87</v>
       </c>
       <c r="K42" s="11" t="s">
         <v>213</v>
@@ -3461,11 +3461,11 @@
       </c>
       <c r="I43" s="9">
         <f ca="1">ROUND(RAND()*(2-1)+1, 2)</f>
-        <v>1.89</v>
+        <v>1.25</v>
       </c>
       <c r="J43" s="9">
         <f ca="1">ROUND(RAND()*(10 -1)+1,2)</f>
-        <v>7.4</v>
+        <v>5.83</v>
       </c>
       <c r="K43" s="9" t="s">
         <v>214</v>
@@ -3513,11 +3513,11 @@
       </c>
       <c r="I44" s="10">
         <f ca="1">ROUND(RAND()*(2-VALUE(I43))+VALUE(I43),2)</f>
-        <v>1.9</v>
+        <v>1.61</v>
       </c>
       <c r="J44" s="10">
         <f ca="1">ROUND(RAND()*(100-VALUE(J43))+VALUE(J43),2)</f>
-        <v>57.07</v>
+        <v>66.42</v>
       </c>
       <c r="K44" s="10" t="s">
         <v>215</v>
@@ -3565,11 +3565,11 @@
       </c>
       <c r="I45" s="9">
         <f ca="1">ROUND(RAND()*(2-1)+1, 2)</f>
-        <v>1.03</v>
+        <v>1.3</v>
       </c>
       <c r="J45" s="9">
         <f t="shared" ref="J45:J50" ca="1" si="0">ROUND(RAND()*(10 -1)+1,2)</f>
-        <v>8.11</v>
+        <v>7.7</v>
       </c>
       <c r="K45" s="11" t="s">
         <v>203</v>
@@ -3617,11 +3617,11 @@
       </c>
       <c r="I46" s="9">
         <f ca="1">ROUND(RAND()*(2-1)+1, 2)</f>
-        <v>1.9</v>
+        <v>1.35</v>
       </c>
       <c r="J46" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>1.26</v>
+        <v>6.66</v>
       </c>
       <c r="K46" s="11" t="s">
         <v>216</v>
@@ -3669,11 +3669,11 @@
       </c>
       <c r="I47" s="9">
         <f ca="1">ROUND(RAND()*(2-1)+1, 2)</f>
-        <v>1.76</v>
+        <v>1.82</v>
       </c>
       <c r="J47" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>7.63</v>
+        <v>7.97</v>
       </c>
       <c r="K47" s="11" t="s">
         <v>217</v>
@@ -3721,11 +3721,11 @@
       </c>
       <c r="I48" s="9">
         <f ca="1">ROUND(RAND()*(2-1)+1, 2)</f>
-        <v>1.88</v>
+        <v>1.1299999999999999</v>
       </c>
       <c r="J48" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>7.52</v>
+        <v>6.46</v>
       </c>
       <c r="K48" s="11" t="s">
         <v>175</v>
@@ -3773,11 +3773,11 @@
       </c>
       <c r="I49" s="11">
         <f ca="1">ROUND(RAND()*(1.4-1)+1, 2)</f>
-        <v>1.03</v>
+        <v>1.0900000000000001</v>
       </c>
       <c r="J49" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>7.12</v>
+        <v>7.66</v>
       </c>
       <c r="K49" s="11" t="s">
         <v>212</v>
@@ -3825,11 +3825,11 @@
       </c>
       <c r="I50" s="10">
         <f ca="1">ROUND(RAND()*(0.5-0.3)+0.3, 2)</f>
-        <v>0.35</v>
+        <v>0.4</v>
       </c>
       <c r="J50" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>4.9400000000000004</v>
+        <v>9.82</v>
       </c>
       <c r="K50" s="10" t="s">
         <v>176</v>
@@ -3858,408 +3858,948 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B49"/>
+  <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B49"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:F49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.5703125" customWidth="1"/>
+    <col min="5" max="5" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="str">
+        <f>_xlfn.CONCAT("SPECIES_",UPPER(D1))</f>
+        <v>SPECIES_ALIEN</v>
+      </c>
+      <c r="F1" t="str">
+        <f>_xlfn.CONCAT(E1,"    UMETA(DisplayName = '", D1,"')," )</f>
+        <v>SPECIES_ALIEN    UMETA(DisplayName = 'Alien'),</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B2" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" t="str">
+        <f t="shared" ref="E2:E49" si="0">_xlfn.CONCAT("SPECIES_",UPPER(D2))</f>
+        <v>SPECIES_ALIEN_BIG</v>
+      </c>
+      <c r="F2" t="str">
+        <f t="shared" ref="F2:F49" si="1">_xlfn.CONCAT(E2,"    UMETA(DisplayName = '", D2,"')," )</f>
+        <v>SPECIES_ALIEN_BIG    UMETA(DisplayName = 'Alien_Big'),</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" t="str">
+        <f t="shared" si="0"/>
+        <v>SPECIES_BIRB</v>
+      </c>
+      <c r="F3" t="str">
+        <f t="shared" si="1"/>
+        <v>SPECIES_BIRB    UMETA(DisplayName = 'Birb'),</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B4" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" t="str">
+        <f t="shared" si="0"/>
+        <v>SPECIES_BIRB_BIG</v>
+      </c>
+      <c r="F4" t="str">
+        <f t="shared" si="1"/>
+        <v>SPECIES_BIRB_BIG    UMETA(DisplayName = 'Birb_Big'),</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" t="str">
+        <f t="shared" si="0"/>
+        <v>SPECIES_CACTORO</v>
+      </c>
+      <c r="F5" t="str">
+        <f t="shared" si="1"/>
+        <v>SPECIES_CACTORO    UMETA(DisplayName = 'Cactoro'),</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B6" s="4">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" t="str">
+        <f t="shared" si="0"/>
+        <v>SPECIES_CACTORO_BIG</v>
+      </c>
+      <c r="F6" t="str">
+        <f t="shared" si="1"/>
+        <v>SPECIES_CACTORO_BIG    UMETA(DisplayName = 'Cactoro_Big'),</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="2">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" t="str">
+        <f t="shared" si="0"/>
+        <v>SPECIES_FISH</v>
+      </c>
+      <c r="F7" t="str">
+        <f t="shared" si="1"/>
+        <v>SPECIES_FISH    UMETA(DisplayName = 'Fish'),</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B8" s="4">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" t="str">
+        <f t="shared" si="0"/>
+        <v>SPECIES_FISH_BIG</v>
+      </c>
+      <c r="F8" t="str">
+        <f t="shared" si="1"/>
+        <v>SPECIES_FISH_BIG    UMETA(DisplayName = 'Fish_Big'),</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="2">
         <v>9</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" t="str">
+        <f t="shared" si="0"/>
+        <v>SPECIES_GREENBLOB</v>
+      </c>
+      <c r="F9" t="str">
+        <f t="shared" si="1"/>
+        <v>SPECIES_GREENBLOB    UMETA(DisplayName = 'GreenBlob'),</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="4">
         <v>10</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" t="str">
+        <f t="shared" si="0"/>
+        <v>SPECIES_GREENSPIKYBLOB</v>
+      </c>
+      <c r="F10" t="str">
+        <f t="shared" si="1"/>
+        <v>SPECIES_GREENSPIKYBLOB    UMETA(DisplayName = 'GreenSpikyBlob'),</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B11" s="2">
         <v>11</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" t="str">
+        <f t="shared" si="0"/>
+        <v>SPECIES_MUSHNUB</v>
+      </c>
+      <c r="F11" t="str">
+        <f t="shared" si="1"/>
+        <v>SPECIES_MUSHNUB    UMETA(DisplayName = 'Mushnub'),</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>9</v>
       </c>
       <c r="B12" s="6">
         <v>12</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" t="str">
+        <f t="shared" si="0"/>
+        <v>SPECIES_MUSHNUB_EVOLVED</v>
+      </c>
+      <c r="F12" t="str">
+        <f t="shared" si="1"/>
+        <v>SPECIES_MUSHNUB_EVOLVED    UMETA(DisplayName = 'Mushnub_Evolved'),</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>27</v>
       </c>
       <c r="B13" s="4">
         <v>13</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D13" t="s">
+        <v>27</v>
+      </c>
+      <c r="E13" t="str">
+        <f t="shared" si="0"/>
+        <v>SPECIES_MUSHROOMKING_BIG</v>
+      </c>
+      <c r="F13" t="str">
+        <f t="shared" si="1"/>
+        <v>SPECIES_MUSHROOMKING_BIG    UMETA(DisplayName = 'MushroomKing_Big'),</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B14" s="2">
         <v>14</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E14" t="str">
+        <f t="shared" si="0"/>
+        <v>SPECIES_YETI</v>
+      </c>
+      <c r="F14" t="str">
+        <f t="shared" si="1"/>
+        <v>SPECIES_YETI    UMETA(DisplayName = 'Yeti'),</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>32</v>
       </c>
       <c r="B15" s="4">
         <v>15</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D15" t="s">
+        <v>32</v>
+      </c>
+      <c r="E15" t="str">
+        <f t="shared" si="0"/>
+        <v>SPECIES_YETI_BIG</v>
+      </c>
+      <c r="F15" t="str">
+        <f t="shared" si="1"/>
+        <v>SPECIES_YETI_BIG    UMETA(DisplayName = 'Yeti_Big'),</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B16" s="2">
         <v>16</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D16" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" t="str">
+        <f t="shared" si="0"/>
+        <v>SPECIES_NINJA</v>
+      </c>
+      <c r="F16" t="str">
+        <f t="shared" si="1"/>
+        <v>SPECIES_NINJA    UMETA(DisplayName = 'Ninja'),</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>28</v>
       </c>
       <c r="B17" s="4">
         <v>17</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D17" t="s">
+        <v>28</v>
+      </c>
+      <c r="E17" t="str">
+        <f t="shared" si="0"/>
+        <v>SPECIES_NINJA_BIG</v>
+      </c>
+      <c r="F17" t="str">
+        <f t="shared" si="1"/>
+        <v>SPECIES_NINJA_BIG    UMETA(DisplayName = 'Ninja_Big'),</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B18" s="2">
         <v>18</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D18" t="s">
+        <v>12</v>
+      </c>
+      <c r="E18" t="str">
+        <f t="shared" si="0"/>
+        <v>SPECIES_ORC</v>
+      </c>
+      <c r="F18" t="str">
+        <f t="shared" si="1"/>
+        <v>SPECIES_ORC    UMETA(DisplayName = 'Orc'),</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>29</v>
       </c>
       <c r="B19" s="6">
         <v>19</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D19" t="s">
+        <v>29</v>
+      </c>
+      <c r="E19" t="str">
+        <f t="shared" si="0"/>
+        <v>SPECIES_ORC_BIG</v>
+      </c>
+      <c r="F19" t="str">
+        <f t="shared" si="1"/>
+        <v>SPECIES_ORC_BIG    UMETA(DisplayName = 'Orc_Big'),</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B20" s="4">
         <v>20</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D20" t="s">
+        <v>30</v>
+      </c>
+      <c r="E20" t="str">
+        <f t="shared" si="0"/>
+        <v>SPECIES_ORC_SKULL_BIG</v>
+      </c>
+      <c r="F20" t="str">
+        <f t="shared" si="1"/>
+        <v>SPECIES_ORC_SKULL_BIG    UMETA(DisplayName = 'Orc_Skull_Big'),</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B21" s="2">
         <v>21</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D21" t="s">
+        <v>13</v>
+      </c>
+      <c r="E21" t="str">
+        <f t="shared" si="0"/>
+        <v>SPECIES_PIGEON</v>
+      </c>
+      <c r="F21" t="str">
+        <f t="shared" si="1"/>
+        <v>SPECIES_PIGEON    UMETA(DisplayName = 'Pigeon'),</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>47</v>
       </c>
       <c r="B22" s="4">
         <v>22</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D22" t="s">
+        <v>47</v>
+      </c>
+      <c r="E22" t="str">
+        <f t="shared" si="0"/>
+        <v>SPECIES_PIGEON_FLYING</v>
+      </c>
+      <c r="F22" t="str">
+        <f t="shared" si="1"/>
+        <v>SPECIES_PIGEON_FLYING    UMETA(DisplayName = 'Pigeon_Flying'),</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B23" s="2">
         <v>23</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D23" t="s">
+        <v>14</v>
+      </c>
+      <c r="E23" t="str">
+        <f t="shared" si="0"/>
+        <v>SPECIES_PINKBLOB</v>
+      </c>
+      <c r="F23" t="str">
+        <f t="shared" si="1"/>
+        <v>SPECIES_PINKBLOB    UMETA(DisplayName = 'PinkBlob'),</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>48</v>
       </c>
       <c r="B24" s="4">
         <v>24</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D24" t="s">
+        <v>48</v>
+      </c>
+      <c r="E24" t="str">
+        <f t="shared" si="0"/>
+        <v>SPECIES_SQUIDLE_FLYING</v>
+      </c>
+      <c r="F24" t="str">
+        <f t="shared" si="1"/>
+        <v>SPECIES_SQUIDLE_FLYING    UMETA(DisplayName = 'Squidle_Flying'),</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B25" s="2">
         <v>25</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D25" t="s">
+        <v>122</v>
+      </c>
+      <c r="E25" t="str">
+        <f t="shared" si="0"/>
+        <v>SPECIES_ALPAKING_FLYING</v>
+      </c>
+      <c r="F25" t="str">
+        <f t="shared" si="1"/>
+        <v>SPECIES_ALPAKING_FLYING    UMETA(DisplayName = 'Alpaking_Flying'),</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>33</v>
       </c>
       <c r="B26" s="4">
         <v>26</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D26" t="s">
+        <v>123</v>
+      </c>
+      <c r="E26" t="str">
+        <f t="shared" si="0"/>
+        <v>SPECIES_ALPAKING_EVOLVED_FLYING</v>
+      </c>
+      <c r="F26" t="str">
+        <f t="shared" si="1"/>
+        <v>SPECIES_ALPAKING_EVOLVED_FLYING    UMETA(DisplayName = 'Alpaking_Evolved_Flying'),</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B27" s="2">
         <v>27</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D27" t="s">
+        <v>36</v>
+      </c>
+      <c r="E27" t="str">
+        <f t="shared" si="0"/>
+        <v>SPECIES_ARMABEE_FLYING</v>
+      </c>
+      <c r="F27" t="str">
+        <f t="shared" si="1"/>
+        <v>SPECIES_ARMABEE_FLYING    UMETA(DisplayName = 'Armabee_Flying'),</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>35</v>
       </c>
       <c r="B28" s="4">
         <v>28</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D28" t="s">
+        <v>35</v>
+      </c>
+      <c r="E28" t="str">
+        <f t="shared" si="0"/>
+        <v>SPECIES_ARMABEE_EVOLVED_FLYING</v>
+      </c>
+      <c r="F28" t="str">
+        <f t="shared" si="1"/>
+        <v>SPECIES_ARMABEE_EVOLVED_FLYING    UMETA(DisplayName = 'Armabee_Evolved_Flying'),</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>37</v>
       </c>
       <c r="B29" s="2">
         <v>29</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D29" t="s">
+        <v>37</v>
+      </c>
+      <c r="E29" t="str">
+        <f t="shared" si="0"/>
+        <v>SPECIES_DEMON_FLYING</v>
+      </c>
+      <c r="F29" t="str">
+        <f t="shared" si="1"/>
+        <v>SPECIES_DEMON_FLYING    UMETA(DisplayName = 'Demon_Flying'),</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B30" s="4">
         <v>30</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D30" t="s">
+        <v>22</v>
+      </c>
+      <c r="E30" t="str">
+        <f t="shared" si="0"/>
+        <v>SPECIES_DEMON_BIG</v>
+      </c>
+      <c r="F30" t="str">
+        <f t="shared" si="1"/>
+        <v>SPECIES_DEMON_BIG    UMETA(DisplayName = 'Demon_Big'),</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B31" s="2">
         <v>31</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D31" t="s">
+        <v>4</v>
+      </c>
+      <c r="E31" t="str">
+        <f t="shared" si="0"/>
+        <v>SPECIES_CHICKEN</v>
+      </c>
+      <c r="F31" t="str">
+        <f t="shared" si="1"/>
+        <v>SPECIES_CHICKEN    UMETA(DisplayName = 'Chicken'),</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
         <v>39</v>
       </c>
       <c r="B32" s="6">
         <v>32</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D32" t="s">
+        <v>39</v>
+      </c>
+      <c r="E32" t="str">
+        <f t="shared" si="0"/>
+        <v>SPECIES_DRAGON_FLYING</v>
+      </c>
+      <c r="F32" t="str">
+        <f t="shared" si="1"/>
+        <v>SPECIES_DRAGON_FLYING    UMETA(DisplayName = 'Dragon_Flying'),</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>38</v>
       </c>
       <c r="B33" s="4">
         <v>33</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D33" t="s">
+        <v>38</v>
+      </c>
+      <c r="E33" t="str">
+        <f t="shared" si="0"/>
+        <v>SPECIES_DRAGON_EVOLVED_FLYING</v>
+      </c>
+      <c r="F33" t="str">
+        <f t="shared" si="1"/>
+        <v>SPECIES_DRAGON_EVOLVED_FLYING    UMETA(DisplayName = 'Dragon_Evolved_Flying'),</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>40</v>
       </c>
       <c r="B34" s="2">
         <v>34</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D34" t="s">
+        <v>40</v>
+      </c>
+      <c r="E34" t="str">
+        <f t="shared" si="0"/>
+        <v>SPECIES_GHOST_FLYING</v>
+      </c>
+      <c r="F34" t="str">
+        <f t="shared" si="1"/>
+        <v>SPECIES_GHOST_FLYING    UMETA(DisplayName = 'Ghost_Flying'),</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>41</v>
       </c>
       <c r="B35" s="4">
         <v>35</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D35" t="s">
+        <v>41</v>
+      </c>
+      <c r="E35" t="str">
+        <f t="shared" si="0"/>
+        <v>SPECIES_GHOST_SKULL_FLYING</v>
+      </c>
+      <c r="F35" t="str">
+        <f t="shared" si="1"/>
+        <v>SPECIES_GHOST_SKULL_FLYING    UMETA(DisplayName = 'Ghost_Skull_Flying'),</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>43</v>
       </c>
       <c r="B36" s="2">
         <v>36</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D36" t="s">
+        <v>43</v>
+      </c>
+      <c r="E36" t="str">
+        <f t="shared" si="0"/>
+        <v>SPECIES_GLUB_FLYING</v>
+      </c>
+      <c r="F36" t="str">
+        <f t="shared" si="1"/>
+        <v>SPECIES_GLUB_FLYING    UMETA(DisplayName = 'Glub_Flying'),</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>42</v>
       </c>
       <c r="B37" s="4">
         <v>37</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D37" t="s">
+        <v>42</v>
+      </c>
+      <c r="E37" t="str">
+        <f t="shared" si="0"/>
+        <v>SPECIES_GLUB_EVOLVED_FLYING</v>
+      </c>
+      <c r="F37" t="str">
+        <f t="shared" si="1"/>
+        <v>SPECIES_GLUB_EVOLVED_FLYING    UMETA(DisplayName = 'Glub_Evolved_Flying'),</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>44</v>
       </c>
       <c r="B38" s="2">
         <v>38</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D38" t="s">
+        <v>44</v>
+      </c>
+      <c r="E38" t="str">
+        <f t="shared" si="0"/>
+        <v>SPECIES_GOLELING_FLYING</v>
+      </c>
+      <c r="F38" t="str">
+        <f t="shared" si="1"/>
+        <v>SPECIES_GOLELING_FLYING    UMETA(DisplayName = 'Goleling_Flying'),</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>45</v>
       </c>
       <c r="B39" s="4">
         <v>39</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D39" t="s">
+        <v>45</v>
+      </c>
+      <c r="E39" t="str">
+        <f t="shared" si="0"/>
+        <v>SPECIES_GOLELING_EVOLVED_FLYING</v>
+      </c>
+      <c r="F39" t="str">
+        <f t="shared" si="1"/>
+        <v>SPECIES_GOLELING_EVOLVED_FLYING    UMETA(DisplayName = 'Goleling_Evolved_Flying'),</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B40" s="8">
         <v>40</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D40" t="s">
+        <v>3</v>
+      </c>
+      <c r="E40" t="str">
+        <f t="shared" si="0"/>
+        <v>SPECIES_CAT</v>
+      </c>
+      <c r="F40" t="str">
+        <f t="shared" si="1"/>
+        <v>SPECIES_CAT    UMETA(DisplayName = 'Cat'),</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
         <v>5</v>
       </c>
       <c r="B41" s="8">
         <v>41</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D41" t="s">
+        <v>5</v>
+      </c>
+      <c r="E41" t="str">
+        <f t="shared" si="0"/>
+        <v>SPECIES_DOG</v>
+      </c>
+      <c r="F41" t="str">
+        <f t="shared" si="1"/>
+        <v>SPECIES_DOG    UMETA(DisplayName = 'Dog'),</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B42" s="2">
         <v>42</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D42" t="s">
+        <v>20</v>
+      </c>
+      <c r="E42" t="str">
+        <f t="shared" si="0"/>
+        <v>SPECIES_BUNNY_BIG</v>
+      </c>
+      <c r="F42" t="str">
+        <f t="shared" si="1"/>
+        <v>SPECIES_BUNNY_BIG    UMETA(DisplayName = 'Bunny_Big'),</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>19</v>
       </c>
       <c r="B43" s="4">
         <v>43</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D43" t="s">
+        <v>19</v>
+      </c>
+      <c r="E43" t="str">
+        <f t="shared" si="0"/>
+        <v>SPECIES_BLUEDEMON_BIG</v>
+      </c>
+      <c r="F43" t="str">
+        <f t="shared" si="1"/>
+        <v>SPECIES_BLUEDEMON_BIG    UMETA(DisplayName = 'BlueDemon_Big'),</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="7" t="s">
         <v>23</v>
       </c>
       <c r="B44" s="8">
         <v>44</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D44" t="s">
+        <v>23</v>
+      </c>
+      <c r="E44" t="str">
+        <f t="shared" si="0"/>
+        <v>SPECIES_DINO_BIG</v>
+      </c>
+      <c r="F44" t="str">
+        <f t="shared" si="1"/>
+        <v>SPECIES_DINO_BIG    UMETA(DisplayName = 'Dino_Big'),</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="7" t="s">
         <v>25</v>
       </c>
       <c r="B45" s="8">
         <v>45</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D45" t="s">
+        <v>25</v>
+      </c>
+      <c r="E45" t="str">
+        <f t="shared" si="0"/>
+        <v>SPECIES_FROG_BIG</v>
+      </c>
+      <c r="F45" t="str">
+        <f t="shared" si="1"/>
+        <v>SPECIES_FROG_BIG    UMETA(DisplayName = 'Frog_Big'),</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="7" t="s">
         <v>26</v>
       </c>
       <c r="B46" s="8">
         <v>46</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D46" t="s">
+        <v>26</v>
+      </c>
+      <c r="E46" t="str">
+        <f t="shared" si="0"/>
+        <v>SPECIES_MONKROOSE_BIG</v>
+      </c>
+      <c r="F46" t="str">
+        <f t="shared" si="1"/>
+        <v>SPECIES_MONKROOSE_BIG    UMETA(DisplayName = 'Monkroose_Big'),</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="7" t="s">
         <v>31</v>
       </c>
       <c r="B47" s="8">
         <v>47</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D47" t="s">
+        <v>31</v>
+      </c>
+      <c r="E47" t="str">
+        <f t="shared" si="0"/>
+        <v>SPECIES_TRIBAL_BIG</v>
+      </c>
+      <c r="F47" t="str">
+        <f t="shared" si="1"/>
+        <v>SPECIES_TRIBAL_BIG    UMETA(DisplayName = 'Tribal_Big'),</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="7" t="s">
         <v>46</v>
       </c>
       <c r="B48" s="8">
         <v>48</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D48" t="s">
+        <v>46</v>
+      </c>
+      <c r="E48" t="str">
+        <f t="shared" si="0"/>
+        <v>SPECIES_HYWIRL_FLYING</v>
+      </c>
+      <c r="F48" t="str">
+        <f t="shared" si="1"/>
+        <v>SPECIES_HYWIRL_FLYING    UMETA(DisplayName = 'Hywirl_Flying'),</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="s">
         <v>15</v>
       </c>
       <c r="B49" s="8">
         <v>49</v>
+      </c>
+      <c r="D49" t="s">
+        <v>15</v>
+      </c>
+      <c r="E49" t="str">
+        <f t="shared" si="0"/>
+        <v>SPECIES_WIZARD</v>
+      </c>
+      <c r="F49" t="str">
+        <f t="shared" si="1"/>
+        <v>SPECIES_WIZARD    UMETA(DisplayName = 'Wizard'),</v>
       </c>
     </row>
   </sheetData>

</xml_diff>